<commit_message>
aggiornamento ind retail e test
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/test/RETAIL/test_Ind_Esperienziali_RETAIL.xlsx
+++ b/earlywarning-pom/Document/test/RETAIL/test_Ind_Esperienziali_RETAIL.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="110">
-  <si>
-    <t>SNDG</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="124">
   <si>
     <t># Indicatore</t>
   </si>
@@ -99,30 +96,6 @@
     <t>FORB00_2</t>
   </si>
   <si>
-    <t>0000000000000498</t>
-  </si>
-  <si>
-    <t>0000000000000499</t>
-  </si>
-  <si>
-    <t>0000000000000500</t>
-  </si>
-  <si>
-    <t>0000000000000501</t>
-  </si>
-  <si>
-    <t>0000000000000502</t>
-  </si>
-  <si>
-    <t>0000000000000503</t>
-  </si>
-  <si>
-    <t>0000000000000505</t>
-  </si>
-  <si>
-    <t>0000000000000504</t>
-  </si>
-  <si>
     <t xml:space="preserve">NUM_RATE_IMPAGATE_DIR </t>
   </si>
   <si>
@@ -135,9 +108,6 @@
     <t>SGR000_1</t>
   </si>
   <si>
-    <t>0000000000000506</t>
-  </si>
-  <si>
     <t>NUM_GG_SCADUTO_DIR</t>
   </si>
   <si>
@@ -150,33 +120,6 @@
     <t>FLG_IRIS_GAR_NDG_PROC_CONC</t>
   </si>
   <si>
-    <t>0000000000000507</t>
-  </si>
-  <si>
-    <t>0000000000000508</t>
-  </si>
-  <si>
-    <t>0000000000000509</t>
-  </si>
-  <si>
-    <t>0000000000000510</t>
-  </si>
-  <si>
-    <t>0000000000000511</t>
-  </si>
-  <si>
-    <t>0000000000000512</t>
-  </si>
-  <si>
-    <t>0000000000000513</t>
-  </si>
-  <si>
-    <t>0000000000000514</t>
-  </si>
-  <si>
-    <t>0000000000000515</t>
-  </si>
-  <si>
     <t>FLG_IRIS_SOC_SOFF</t>
   </si>
   <si>
@@ -186,90 +129,12 @@
     <t>FLG_IRIS_SOC_GAR_NEG_ATT</t>
   </si>
   <si>
-    <t>0000000000000516</t>
-  </si>
-  <si>
-    <t>0000000000000517</t>
-  </si>
-  <si>
-    <t>0000000000000518</t>
-  </si>
-  <si>
-    <t>0000000000000519</t>
-  </si>
-  <si>
-    <t>0000000000000520</t>
-  </si>
-  <si>
-    <t>0000000000000521</t>
-  </si>
-  <si>
-    <t>0000000000000522</t>
-  </si>
-  <si>
-    <t>0000000000000523</t>
-  </si>
-  <si>
-    <t>000000000000052</t>
-  </si>
-  <si>
-    <t>0000000000000525</t>
-  </si>
-  <si>
-    <t>0000000000000526</t>
-  </si>
-  <si>
-    <t>0000000000000527</t>
-  </si>
-  <si>
-    <t>0000000000000528</t>
-  </si>
-  <si>
-    <t>0000000000000529</t>
-  </si>
-  <si>
-    <t>0000000000000530</t>
-  </si>
-  <si>
-    <t>0000000000000531</t>
-  </si>
-  <si>
-    <t>0000000000000532</t>
-  </si>
-  <si>
     <t>NUM_RATE_IMPAGATE_RIDMAV</t>
   </si>
   <si>
-    <t>0000000000000533</t>
-  </si>
-  <si>
-    <t>0000000000000534</t>
-  </si>
-  <si>
-    <t>0000000000000535</t>
-  </si>
-  <si>
     <t>NUM_GG_SCADUTO_RIDMAV</t>
   </si>
   <si>
-    <t>0000000000000536</t>
-  </si>
-  <si>
-    <t>0000000000000537</t>
-  </si>
-  <si>
-    <t>0000000000000538</t>
-  </si>
-  <si>
-    <t>0000000000000539</t>
-  </si>
-  <si>
-    <t>0000000000000540</t>
-  </si>
-  <si>
-    <t>0000000000000541</t>
-  </si>
-  <si>
     <t>NUM_RATE_IMP_CDQ</t>
   </si>
   <si>
@@ -282,79 +147,256 @@
     <t>CQU000_2</t>
   </si>
   <si>
-    <t>0000000000000542</t>
-  </si>
-  <si>
-    <t>0000000000000548</t>
-  </si>
-  <si>
-    <t>0000000000000543</t>
-  </si>
-  <si>
     <t>IMP_ARRETRATO_CDQ</t>
   </si>
   <si>
-    <t>0000000000000544</t>
-  </si>
-  <si>
-    <t>0000000000000545</t>
-  </si>
-  <si>
-    <t>0000000000000546</t>
-  </si>
-  <si>
-    <t>0000000000000547</t>
-  </si>
-  <si>
-    <t>0000000000000549</t>
-  </si>
-  <si>
-    <t>0000000000000550</t>
-  </si>
-  <si>
-    <t>0000000000000551</t>
-  </si>
-  <si>
-    <t>0000000000000552</t>
-  </si>
-  <si>
-    <t>0000000000000553</t>
-  </si>
-  <si>
-    <t>0000000000000554</t>
-  </si>
-  <si>
-    <t>0000000000000555</t>
-  </si>
-  <si>
-    <t>0000000000000556</t>
-  </si>
-  <si>
-    <t>0000000000000557</t>
-  </si>
-  <si>
-    <t>0000000000000558</t>
-  </si>
-  <si>
-    <t>0000000000000559</t>
-  </si>
-  <si>
-    <t>0000000000000560</t>
-  </si>
-  <si>
-    <t>0000000000000561</t>
-  </si>
-  <si>
     <t>mising</t>
   </si>
   <si>
     <t>SGR000_2</t>
+  </si>
+  <si>
+    <t>COD_SNDG</t>
+  </si>
+  <si>
+    <t>'0000000000000498'</t>
+  </si>
+  <si>
+    <t>'0000000000000499'</t>
+  </si>
+  <si>
+    <t>'0000000000000500'</t>
+  </si>
+  <si>
+    <t>'0000000000000501'</t>
+  </si>
+  <si>
+    <t>'0000000000000502'</t>
+  </si>
+  <si>
+    <t>'0000000000000503'</t>
+  </si>
+  <si>
+    <t>'0000000000000504'</t>
+  </si>
+  <si>
+    <t>'0000000000000505'</t>
+  </si>
+  <si>
+    <t>'0000000000000506'</t>
+  </si>
+  <si>
+    <t>'0000000000000507'</t>
+  </si>
+  <si>
+    <t>'0000000000000508'</t>
+  </si>
+  <si>
+    <t>'0000000000000509'</t>
+  </si>
+  <si>
+    <t>'0000000000000510'</t>
+  </si>
+  <si>
+    <t>'0000000000000511'</t>
+  </si>
+  <si>
+    <t>'0000000000000512'</t>
+  </si>
+  <si>
+    <t>'0000000000000513'</t>
+  </si>
+  <si>
+    <t>'0000000000000514'</t>
+  </si>
+  <si>
+    <t>'0000000000000515'</t>
+  </si>
+  <si>
+    <t>'0000000000000516'</t>
+  </si>
+  <si>
+    <t>'0000000000000517'</t>
+  </si>
+  <si>
+    <t>'0000000000000518'</t>
+  </si>
+  <si>
+    <t>'0000000000000519'</t>
+  </si>
+  <si>
+    <t>'0000000000000520'</t>
+  </si>
+  <si>
+    <t>'0000000000000521'</t>
+  </si>
+  <si>
+    <t>'0000000000000522'</t>
+  </si>
+  <si>
+    <t>'0000000000000523'</t>
+  </si>
+  <si>
+    <t>'000000000000052 '</t>
+  </si>
+  <si>
+    <t>'0000000000000525'</t>
+  </si>
+  <si>
+    <t>'0000000000000526'</t>
+  </si>
+  <si>
+    <t>'0000000000000527'</t>
+  </si>
+  <si>
+    <t>'0000000000000528'</t>
+  </si>
+  <si>
+    <t>'0000000000000529'</t>
+  </si>
+  <si>
+    <t>'0000000000000530'</t>
+  </si>
+  <si>
+    <t>'0000000000000531'</t>
+  </si>
+  <si>
+    <t>'0000000000000532'</t>
+  </si>
+  <si>
+    <t>'0000000000000533'</t>
+  </si>
+  <si>
+    <t>'0000000000000534'</t>
+  </si>
+  <si>
+    <t>'0000000000000535'</t>
+  </si>
+  <si>
+    <t>'0000000000000536'</t>
+  </si>
+  <si>
+    <t>'0000000000000537'</t>
+  </si>
+  <si>
+    <t>'0000000000000538'</t>
+  </si>
+  <si>
+    <t>'0000000000000539'</t>
+  </si>
+  <si>
+    <t>'0000000000000540'</t>
+  </si>
+  <si>
+    <t>'0000000000000541'</t>
+  </si>
+  <si>
+    <t>'0000000000000542'</t>
+  </si>
+  <si>
+    <t>'0000000000000543'</t>
+  </si>
+  <si>
+    <t>'0000000000000544'</t>
+  </si>
+  <si>
+    <t>'0000000000000545'</t>
+  </si>
+  <si>
+    <t>'0000000000000546'</t>
+  </si>
+  <si>
+    <t>'0000000000000547'</t>
+  </si>
+  <si>
+    <t>'0000000000000548'</t>
+  </si>
+  <si>
+    <t>'0000000000000549'</t>
+  </si>
+  <si>
+    <t>'0000000000000550'</t>
+  </si>
+  <si>
+    <t>'0000000000000551'</t>
+  </si>
+  <si>
+    <t>'0000000000000552'</t>
+  </si>
+  <si>
+    <t>'0000000000000553'</t>
+  </si>
+  <si>
+    <t>'0000000000000554'</t>
+  </si>
+  <si>
+    <t>'0000000000000555'</t>
+  </si>
+  <si>
+    <t>'0000000000000556'</t>
+  </si>
+  <si>
+    <t>'0000000000000557'</t>
+  </si>
+  <si>
+    <t>'0000000000000558'</t>
+  </si>
+  <si>
+    <t>'0000000000000559'</t>
+  </si>
+  <si>
+    <t>'0000000000000560'</t>
+  </si>
+  <si>
+    <t>'0000000000000561'</t>
+  </si>
+  <si>
+    <t>S00</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>200.000000</t>
+  </si>
+  <si>
+    <t>400.000000</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>250.000000</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>FORB000_1</t>
+  </si>
+  <si>
+    <t>FORB000_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -383,7 +425,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,6 +441,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -465,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -518,9 +578,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -832,144 +923,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BB81"/>
+  <dimension ref="A1:BL81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="17.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" style="1" customWidth="1"/>
-    <col min="9" max="11" width="23.44140625" style="1" customWidth="1"/>
-    <col min="12" max="15" width="29.21875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="24.88671875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="20.5546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="19.21875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="28.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" style="1" customWidth="1"/>
+    <col min="9" max="11" width="23.42578125" style="1" customWidth="1"/>
+    <col min="12" max="15" width="29.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="24.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="20.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="19.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="28.42578125" style="1" customWidth="1"/>
     <col min="20" max="20" width="26" style="1" customWidth="1"/>
-    <col min="21" max="24" width="23.21875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.6640625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="47" width="8.88671875" style="1"/>
-    <col min="48" max="50" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="8.88671875" style="1"/>
+    <col min="21" max="24" width="23.28515625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.7109375" style="1" customWidth="1"/>
+    <col min="30" max="30" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.85546875" style="1"/>
+    <col min="32" max="32" width="21" style="1" customWidth="1"/>
+    <col min="33" max="33" width="19.5703125" style="1" customWidth="1"/>
+    <col min="34" max="34" width="36.42578125" style="1" customWidth="1"/>
+    <col min="35" max="35" width="22.42578125" style="1" customWidth="1"/>
+    <col min="36" max="36" width="29.28515625" style="1" customWidth="1"/>
+    <col min="37" max="47" width="8.85546875" style="1"/>
+    <col min="48" max="50" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:31" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="AB1" s="18"/>
+    </row>
+    <row r="2" spans="1:64" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AE2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5"/>
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="5"/>
+      <c r="AQ2" s="5"/>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="5"/>
+      <c r="AU2" s="5"/>
+      <c r="AV2" s="5"/>
+      <c r="AW2" s="5"/>
+      <c r="AX2" s="5"/>
+      <c r="AY2" s="5"/>
+      <c r="AZ2" s="5"/>
+      <c r="BA2" s="5"/>
+      <c r="BB2" s="5"/>
+      <c r="BC2" s="27"/>
+      <c r="BD2" s="27"/>
+      <c r="BE2" s="27"/>
+      <c r="BF2" s="27"/>
+    </row>
+    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C3" s="6">
         <v>100</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6">
@@ -999,19 +1126,56 @@
       <c r="Z3" s="6"/>
       <c r="AA3" s="6"/>
       <c r="AB3" s="6"/>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="3"/>
-      <c r="AE3" s="3"/>
-    </row>
-    <row r="4" spans="1:31" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF3" s="28"/>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="5"/>
+      <c r="AI3" s="5"/>
+      <c r="AJ3" s="5"/>
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="5"/>
+      <c r="AM3" s="5"/>
+      <c r="AN3" s="5"/>
+      <c r="AO3" s="5"/>
+      <c r="AP3" s="5"/>
+      <c r="AQ3" s="5"/>
+      <c r="AR3" s="5"/>
+      <c r="AS3" s="5"/>
+      <c r="AT3" s="5"/>
+      <c r="AU3" s="5"/>
+      <c r="AV3" s="5"/>
+      <c r="AW3" s="5"/>
+      <c r="AX3" s="5"/>
+      <c r="AY3" s="5"/>
+      <c r="AZ3" s="5"/>
+      <c r="BA3" s="5"/>
+      <c r="BB3" s="5"/>
+      <c r="BC3" s="5"/>
+      <c r="BD3" s="5"/>
+      <c r="BE3" s="28"/>
+      <c r="BF3" s="5"/>
+      <c r="BG3" s="1"/>
+      <c r="BH3" s="1"/>
+      <c r="BI3" s="1"/>
+      <c r="BJ3" s="1"/>
+      <c r="BK3" s="1"/>
+      <c r="BL3" s="1"/>
+    </row>
+    <row r="4" spans="1:64" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C4" s="6">
         <v>100</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6">
@@ -1041,28 +1205,59 @@
       <c r="Z4" s="6"/>
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
-      <c r="AC4" s="3"/>
-      <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AC4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF4" s="28"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="5"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="5"/>
+      <c r="AN4" s="5"/>
+      <c r="AO4" s="5"/>
+      <c r="AP4" s="5"/>
+      <c r="AQ4" s="5"/>
+      <c r="AR4" s="5"/>
+      <c r="AS4" s="5"/>
+      <c r="AT4" s="5"/>
+      <c r="AU4" s="5"/>
+      <c r="AV4" s="5"/>
+      <c r="AW4" s="5"/>
+      <c r="AX4" s="5"/>
+      <c r="AY4" s="5"/>
+      <c r="AZ4" s="5"/>
+      <c r="BA4" s="5"/>
+      <c r="BB4" s="5"/>
+      <c r="BC4" s="5"/>
+      <c r="BD4" s="5"/>
+      <c r="BE4" s="28"/>
+      <c r="BF4" s="27"/>
+    </row>
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="C5" s="6">
         <v>100</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -1085,23 +1280,56 @@
       <c r="Z5" s="6"/>
       <c r="AA5" s="6"/>
       <c r="AB5" s="6"/>
-      <c r="AC5" s="3"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AC5" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AD5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF5" s="28"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="5"/>
+      <c r="AQ5" s="5"/>
+      <c r="AR5" s="5"/>
+      <c r="AS5" s="5"/>
+      <c r="AT5" s="5"/>
+      <c r="AU5" s="5"/>
+      <c r="AV5" s="5"/>
+      <c r="AW5" s="5"/>
+      <c r="AX5" s="5"/>
+      <c r="AY5" s="5"/>
+      <c r="AZ5" s="5"/>
+      <c r="BA5" s="5"/>
+      <c r="BB5" s="5"/>
+      <c r="BC5" s="5"/>
+      <c r="BD5" s="5"/>
+      <c r="BE5" s="28"/>
+      <c r="BF5" s="27"/>
+    </row>
+    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C6" s="6">
         <v>100</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" s="6">
         <v>1</v>
@@ -1127,26 +1355,57 @@
       <c r="Z6" s="6"/>
       <c r="AA6" s="6"/>
       <c r="AB6" s="6"/>
-      <c r="AC6" s="3"/>
-      <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AC6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF6" s="28"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="5"/>
+      <c r="AM6" s="5"/>
+      <c r="AN6" s="5"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="5"/>
+      <c r="AQ6" s="5"/>
+      <c r="AR6" s="5"/>
+      <c r="AS6" s="5"/>
+      <c r="AT6" s="5"/>
+      <c r="AU6" s="5"/>
+      <c r="AV6" s="5"/>
+      <c r="AW6" s="5"/>
+      <c r="AX6" s="5"/>
+      <c r="AY6" s="5"/>
+      <c r="AZ6" s="5"/>
+      <c r="BA6" s="5"/>
+      <c r="BB6" s="5"/>
+      <c r="BC6" s="5"/>
+      <c r="BD6" s="5"/>
+      <c r="BE6" s="28"/>
+      <c r="BF6" s="27"/>
+    </row>
+    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C7" s="6">
         <v>100</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6">
         <v>1</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -1169,23 +1428,54 @@
       <c r="Z7" s="6"/>
       <c r="AA7" s="6"/>
       <c r="AB7" s="6"/>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
-      <c r="AE7" s="3"/>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AC7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF7" s="28"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="5"/>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="5"/>
+      <c r="AM7" s="5"/>
+      <c r="AN7" s="5"/>
+      <c r="AO7" s="5"/>
+      <c r="AP7" s="5"/>
+      <c r="AQ7" s="5"/>
+      <c r="AR7" s="5"/>
+      <c r="AS7" s="5"/>
+      <c r="AT7" s="5"/>
+      <c r="AU7" s="5"/>
+      <c r="AV7" s="5"/>
+      <c r="AW7" s="5"/>
+      <c r="AX7" s="5"/>
+      <c r="AY7" s="5"/>
+      <c r="AZ7" s="5"/>
+      <c r="BA7" s="5"/>
+      <c r="BB7" s="5"/>
+      <c r="BC7" s="5"/>
+      <c r="BD7" s="5"/>
+      <c r="BE7" s="28"/>
+      <c r="BF7" s="27"/>
+    </row>
+    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="4" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C8" s="6">
         <v>100</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>17</v>
+        <v>43</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="F8" s="6">
         <v>0</v>
@@ -1214,20 +1504,53 @@
       <c r="Z8" s="6"/>
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
-      <c r="AE8" s="3"/>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AC8" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AD8" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE8" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF8" s="28"/>
+      <c r="AG8" s="5"/>
+      <c r="AH8" s="5"/>
+      <c r="AI8" s="5"/>
+      <c r="AJ8" s="5"/>
+      <c r="AK8" s="5"/>
+      <c r="AL8" s="5"/>
+      <c r="AM8" s="5"/>
+      <c r="AN8" s="5"/>
+      <c r="AO8" s="5"/>
+      <c r="AP8" s="5"/>
+      <c r="AQ8" s="5"/>
+      <c r="AR8" s="5"/>
+      <c r="AS8" s="5"/>
+      <c r="AT8" s="5"/>
+      <c r="AU8" s="5"/>
+      <c r="AV8" s="5"/>
+      <c r="AW8" s="5"/>
+      <c r="AX8" s="5"/>
+      <c r="AY8" s="5"/>
+      <c r="AZ8" s="5"/>
+      <c r="BA8" s="5"/>
+      <c r="BB8" s="5"/>
+      <c r="BC8" s="5"/>
+      <c r="BD8" s="5"/>
+      <c r="BE8" s="28"/>
+      <c r="BF8" s="27"/>
+    </row>
+    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="4" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="C9" s="6">
         <v>100</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6">
@@ -1257,14 +1580,45 @@
       <c r="Z9" s="6"/>
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
-      <c r="AC9" s="3"/>
-      <c r="AD9" s="3"/>
-      <c r="AE9" s="3"/>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AC9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF9" s="28"/>
+      <c r="AG9" s="5"/>
+      <c r="AH9" s="5"/>
+      <c r="AI9" s="5"/>
+      <c r="AJ9" s="5"/>
+      <c r="AK9" s="5"/>
+      <c r="AL9" s="5"/>
+      <c r="AM9" s="5"/>
+      <c r="AN9" s="5"/>
+      <c r="AO9" s="5"/>
+      <c r="AP9" s="5"/>
+      <c r="AQ9" s="5"/>
+      <c r="AR9" s="5"/>
+      <c r="AS9" s="5"/>
+      <c r="AT9" s="5"/>
+      <c r="AU9" s="5"/>
+      <c r="AV9" s="5"/>
+      <c r="AW9" s="5"/>
+      <c r="AX9" s="5"/>
+      <c r="AY9" s="5"/>
+      <c r="AZ9" s="5"/>
+      <c r="BA9" s="5"/>
+      <c r="BB9" s="5"/>
+      <c r="BC9" s="5"/>
+      <c r="BD9" s="5"/>
+      <c r="BE9" s="28"/>
+      <c r="BF9" s="27"/>
+    </row>
+    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="4" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C10" s="6">
         <v>101</v>
@@ -1301,28 +1655,57 @@
       <c r="Z10" s="6"/>
       <c r="AA10" s="6"/>
       <c r="AB10" s="6"/>
-      <c r="AC10" s="3"/>
-      <c r="AD10" s="3"/>
+      <c r="AC10" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="AD10" s="6"/>
       <c r="AE10" s="3"/>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF10" s="28"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="5"/>
+      <c r="AI10" s="5"/>
+      <c r="AJ10" s="5"/>
+      <c r="AK10" s="5"/>
+      <c r="AL10" s="5"/>
+      <c r="AM10" s="5"/>
+      <c r="AN10" s="5"/>
+      <c r="AO10" s="5"/>
+      <c r="AP10" s="5"/>
+      <c r="AQ10" s="5"/>
+      <c r="AR10" s="5"/>
+      <c r="AS10" s="5"/>
+      <c r="AT10" s="5"/>
+      <c r="AU10" s="5"/>
+      <c r="AV10" s="5"/>
+      <c r="AW10" s="5"/>
+      <c r="AX10" s="5"/>
+      <c r="AY10" s="5"/>
+      <c r="AZ10" s="5"/>
+      <c r="BA10" s="5"/>
+      <c r="BB10" s="5"/>
+      <c r="BC10" s="5"/>
+      <c r="BD10" s="5"/>
+      <c r="BE10" s="28"/>
+      <c r="BF10" s="27"/>
+    </row>
+    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="4" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C11" s="6">
         <v>101</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11" s="6">
         <v>300</v>
@@ -1346,23 +1729,54 @@
       <c r="Z11" s="6"/>
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
-      <c r="AC11" s="3"/>
-      <c r="AD11" s="3"/>
+      <c r="AC11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD11" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="AE11" s="3"/>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF11" s="28"/>
+      <c r="AG11" s="5"/>
+      <c r="AH11" s="5"/>
+      <c r="AI11" s="5"/>
+      <c r="AJ11" s="5"/>
+      <c r="AK11" s="5"/>
+      <c r="AL11" s="5"/>
+      <c r="AM11" s="5"/>
+      <c r="AN11" s="5"/>
+      <c r="AO11" s="5"/>
+      <c r="AP11" s="5"/>
+      <c r="AQ11" s="5"/>
+      <c r="AR11" s="5"/>
+      <c r="AS11" s="5"/>
+      <c r="AT11" s="5"/>
+      <c r="AU11" s="5"/>
+      <c r="AV11" s="5"/>
+      <c r="AW11" s="5"/>
+      <c r="AX11" s="5"/>
+      <c r="AY11" s="5"/>
+      <c r="AZ11" s="5"/>
+      <c r="BA11" s="5"/>
+      <c r="BB11" s="5"/>
+      <c r="BC11" s="5"/>
+      <c r="BD11" s="5"/>
+      <c r="BE11" s="28"/>
+      <c r="BF11" s="27"/>
+    </row>
+    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="4" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="C12" s="6">
         <v>101</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -1370,7 +1784,7 @@
         <v>300</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
@@ -1391,31 +1805,62 @@
       <c r="Z12" s="6"/>
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
-      <c r="AC12" s="3"/>
-      <c r="AD12" s="3"/>
+      <c r="AC12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD12" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="AE12" s="3"/>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF12" s="28"/>
+      <c r="AG12" s="5"/>
+      <c r="AH12" s="5"/>
+      <c r="AI12" s="5"/>
+      <c r="AJ12" s="5"/>
+      <c r="AK12" s="5"/>
+      <c r="AL12" s="5"/>
+      <c r="AM12" s="5"/>
+      <c r="AN12" s="5"/>
+      <c r="AO12" s="5"/>
+      <c r="AP12" s="5"/>
+      <c r="AQ12" s="5"/>
+      <c r="AR12" s="5"/>
+      <c r="AS12" s="5"/>
+      <c r="AT12" s="5"/>
+      <c r="AU12" s="5"/>
+      <c r="AV12" s="5"/>
+      <c r="AW12" s="5"/>
+      <c r="AX12" s="5"/>
+      <c r="AY12" s="5"/>
+      <c r="AZ12" s="5"/>
+      <c r="BA12" s="5"/>
+      <c r="BB12" s="5"/>
+      <c r="BC12" s="5"/>
+      <c r="BD12" s="5"/>
+      <c r="BE12" s="28"/>
+      <c r="BF12" s="27"/>
+    </row>
+    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="4" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="C13" s="6">
         <v>101</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -1436,23 +1881,54 @@
       <c r="Z13" s="6"/>
       <c r="AA13" s="6"/>
       <c r="AB13" s="6"/>
-      <c r="AC13" s="3"/>
-      <c r="AD13" s="3"/>
+      <c r="AC13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD13" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="AE13" s="3"/>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF13" s="28"/>
+      <c r="AG13" s="5"/>
+      <c r="AH13" s="5"/>
+      <c r="AI13" s="5"/>
+      <c r="AJ13" s="5"/>
+      <c r="AK13" s="5"/>
+      <c r="AL13" s="5"/>
+      <c r="AM13" s="5"/>
+      <c r="AN13" s="5"/>
+      <c r="AO13" s="5"/>
+      <c r="AP13" s="5"/>
+      <c r="AQ13" s="5"/>
+      <c r="AR13" s="5"/>
+      <c r="AS13" s="5"/>
+      <c r="AT13" s="5"/>
+      <c r="AU13" s="5"/>
+      <c r="AV13" s="5"/>
+      <c r="AW13" s="5"/>
+      <c r="AX13" s="5"/>
+      <c r="AY13" s="5"/>
+      <c r="AZ13" s="5"/>
+      <c r="BA13" s="5"/>
+      <c r="BB13" s="5"/>
+      <c r="BC13" s="5"/>
+      <c r="BD13" s="5"/>
+      <c r="BE13" s="28"/>
+      <c r="BF13" s="27"/>
+    </row>
+    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="4" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C14" s="6">
         <v>101</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>109</v>
+      <c r="D14" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -1481,14 +1957,43 @@
       <c r="Z14" s="6"/>
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
-      <c r="AC14" s="3"/>
-      <c r="AD14" s="3"/>
+      <c r="AC14" s="20">
+        <v>-2</v>
+      </c>
+      <c r="AD14" s="19"/>
       <c r="AE14" s="3"/>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF14" s="28"/>
+      <c r="AG14" s="5"/>
+      <c r="AH14" s="5"/>
+      <c r="AI14" s="5"/>
+      <c r="AJ14" s="5"/>
+      <c r="AK14" s="5"/>
+      <c r="AL14" s="5"/>
+      <c r="AM14" s="5"/>
+      <c r="AN14" s="5"/>
+      <c r="AO14" s="5"/>
+      <c r="AP14" s="5"/>
+      <c r="AQ14" s="5"/>
+      <c r="AR14" s="5"/>
+      <c r="AS14" s="5"/>
+      <c r="AT14" s="5"/>
+      <c r="AU14" s="5"/>
+      <c r="AV14" s="5"/>
+      <c r="AW14" s="5"/>
+      <c r="AX14" s="5"/>
+      <c r="AY14" s="5"/>
+      <c r="AZ14" s="5"/>
+      <c r="BA14" s="5"/>
+      <c r="BB14" s="5"/>
+      <c r="BC14" s="5"/>
+      <c r="BD14" s="5"/>
+      <c r="BE14" s="28"/>
+      <c r="BF14" s="27"/>
+    </row>
+    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="4" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C15" s="6">
         <v>102</v>
@@ -1522,14 +2027,43 @@
       <c r="Z15" s="6"/>
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
-      <c r="AC15" s="3"/>
+      <c r="AC15" s="6">
+        <v>1</v>
+      </c>
       <c r="AD15" s="3"/>
       <c r="AE15" s="3"/>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF15" s="28"/>
+      <c r="AG15" s="5"/>
+      <c r="AH15" s="5"/>
+      <c r="AI15" s="5"/>
+      <c r="AJ15" s="5"/>
+      <c r="AK15" s="5"/>
+      <c r="AL15" s="5"/>
+      <c r="AM15" s="5"/>
+      <c r="AN15" s="5"/>
+      <c r="AO15" s="5"/>
+      <c r="AP15" s="5"/>
+      <c r="AQ15" s="5"/>
+      <c r="AR15" s="5"/>
+      <c r="AS15" s="5"/>
+      <c r="AT15" s="5"/>
+      <c r="AU15" s="5"/>
+      <c r="AV15" s="5"/>
+      <c r="AW15" s="5"/>
+      <c r="AX15" s="5"/>
+      <c r="AY15" s="5"/>
+      <c r="AZ15" s="5"/>
+      <c r="BA15" s="5"/>
+      <c r="BB15" s="5"/>
+      <c r="BC15" s="5"/>
+      <c r="BD15" s="5"/>
+      <c r="BE15" s="28"/>
+      <c r="BF15" s="27"/>
+    </row>
+    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="4" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C16" s="6">
         <v>102</v>
@@ -1563,30 +2097,59 @@
       <c r="Z16" s="6"/>
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
-      <c r="AC16" s="3"/>
+      <c r="AC16" s="6">
+        <v>0</v>
+      </c>
       <c r="AD16" s="3"/>
       <c r="AE16" s="3"/>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF16" s="28"/>
+      <c r="AG16" s="5"/>
+      <c r="AH16" s="5"/>
+      <c r="AI16" s="5"/>
+      <c r="AJ16" s="5"/>
+      <c r="AK16" s="5"/>
+      <c r="AL16" s="5"/>
+      <c r="AM16" s="5"/>
+      <c r="AN16" s="5"/>
+      <c r="AO16" s="5"/>
+      <c r="AP16" s="5"/>
+      <c r="AQ16" s="5"/>
+      <c r="AR16" s="5"/>
+      <c r="AS16" s="5"/>
+      <c r="AT16" s="5"/>
+      <c r="AU16" s="5"/>
+      <c r="AV16" s="5"/>
+      <c r="AW16" s="5"/>
+      <c r="AX16" s="5"/>
+      <c r="AY16" s="5"/>
+      <c r="AZ16" s="5"/>
+      <c r="BA16" s="5"/>
+      <c r="BB16" s="5"/>
+      <c r="BC16" s="5"/>
+      <c r="BD16" s="5"/>
+      <c r="BE16" s="28"/>
+      <c r="BF16" s="27"/>
+    </row>
+    <row r="17" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="4" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C17" s="6">
         <v>102</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>37</v>
+      <c r="D17" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>28</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
@@ -1606,14 +2169,45 @@
       <c r="Z17" s="6"/>
       <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
-      <c r="AC17" s="3"/>
-      <c r="AD17" s="3"/>
+      <c r="AC17" s="20">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="AE17" s="3"/>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF17" s="28"/>
+      <c r="AG17" s="5"/>
+      <c r="AH17" s="5"/>
+      <c r="AI17" s="5"/>
+      <c r="AJ17" s="5"/>
+      <c r="AK17" s="5"/>
+      <c r="AL17" s="5"/>
+      <c r="AM17" s="5"/>
+      <c r="AN17" s="5"/>
+      <c r="AO17" s="5"/>
+      <c r="AP17" s="5"/>
+      <c r="AQ17" s="5"/>
+      <c r="AR17" s="5"/>
+      <c r="AS17" s="5"/>
+      <c r="AT17" s="5"/>
+      <c r="AU17" s="5"/>
+      <c r="AV17" s="5"/>
+      <c r="AW17" s="5"/>
+      <c r="AX17" s="5"/>
+      <c r="AY17" s="5"/>
+      <c r="AZ17" s="5"/>
+      <c r="BA17" s="5"/>
+      <c r="BB17" s="5"/>
+      <c r="BC17" s="5"/>
+      <c r="BD17" s="5"/>
+      <c r="BE17" s="28"/>
+      <c r="BF17" s="27"/>
+    </row>
+    <row r="18" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="4" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C18" s="6">
         <v>103</v>
@@ -1649,14 +2243,43 @@
       <c r="Z18" s="6"/>
       <c r="AA18" s="6"/>
       <c r="AB18" s="6"/>
-      <c r="AC18" s="3"/>
-      <c r="AD18" s="3"/>
+      <c r="AC18" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD18" s="7"/>
       <c r="AE18" s="3"/>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF18" s="28"/>
+      <c r="AG18" s="5"/>
+      <c r="AH18" s="5"/>
+      <c r="AI18" s="5"/>
+      <c r="AJ18" s="5"/>
+      <c r="AK18" s="5"/>
+      <c r="AL18" s="5"/>
+      <c r="AM18" s="5"/>
+      <c r="AN18" s="5"/>
+      <c r="AO18" s="5"/>
+      <c r="AP18" s="5"/>
+      <c r="AQ18" s="5"/>
+      <c r="AR18" s="5"/>
+      <c r="AS18" s="5"/>
+      <c r="AT18" s="5"/>
+      <c r="AU18" s="5"/>
+      <c r="AV18" s="5"/>
+      <c r="AW18" s="5"/>
+      <c r="AX18" s="5"/>
+      <c r="AY18" s="5"/>
+      <c r="AZ18" s="5"/>
+      <c r="BA18" s="5"/>
+      <c r="BB18" s="5"/>
+      <c r="BC18" s="5"/>
+      <c r="BD18" s="5"/>
+      <c r="BE18" s="28"/>
+      <c r="BF18" s="27"/>
+    </row>
+    <row r="19" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="4" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C19" s="6">
         <v>103</v>
@@ -1692,14 +2315,43 @@
       <c r="Z19" s="6"/>
       <c r="AA19" s="6"/>
       <c r="AB19" s="6"/>
-      <c r="AC19" s="3"/>
-      <c r="AD19" s="3"/>
+      <c r="AC19" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD19" s="7"/>
       <c r="AE19" s="3"/>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF19" s="28"/>
+      <c r="AG19" s="5"/>
+      <c r="AH19" s="5"/>
+      <c r="AI19" s="5"/>
+      <c r="AJ19" s="5"/>
+      <c r="AK19" s="5"/>
+      <c r="AL19" s="5"/>
+      <c r="AM19" s="5"/>
+      <c r="AN19" s="5"/>
+      <c r="AO19" s="5"/>
+      <c r="AP19" s="5"/>
+      <c r="AQ19" s="5"/>
+      <c r="AR19" s="5"/>
+      <c r="AS19" s="5"/>
+      <c r="AT19" s="5"/>
+      <c r="AU19" s="5"/>
+      <c r="AV19" s="5"/>
+      <c r="AW19" s="5"/>
+      <c r="AX19" s="5"/>
+      <c r="AY19" s="5"/>
+      <c r="AZ19" s="5"/>
+      <c r="BA19" s="5"/>
+      <c r="BB19" s="5"/>
+      <c r="BC19" s="5"/>
+      <c r="BD19" s="5"/>
+      <c r="BE19" s="28"/>
+      <c r="BF19" s="27"/>
+    </row>
+    <row r="20" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="4" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C20" s="6">
         <v>103</v>
@@ -1717,7 +2369,7 @@
         <v>1</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
@@ -1735,14 +2387,43 @@
       <c r="Z20" s="6"/>
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
-      <c r="AC20" s="3"/>
-      <c r="AD20" s="3"/>
+      <c r="AC20" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD20" s="7"/>
       <c r="AE20" s="3"/>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF20" s="28"/>
+      <c r="AG20" s="5"/>
+      <c r="AH20" s="5"/>
+      <c r="AI20" s="5"/>
+      <c r="AJ20" s="5"/>
+      <c r="AK20" s="5"/>
+      <c r="AL20" s="5"/>
+      <c r="AM20" s="5"/>
+      <c r="AN20" s="5"/>
+      <c r="AO20" s="5"/>
+      <c r="AP20" s="5"/>
+      <c r="AQ20" s="5"/>
+      <c r="AR20" s="5"/>
+      <c r="AS20" s="5"/>
+      <c r="AT20" s="5"/>
+      <c r="AU20" s="5"/>
+      <c r="AV20" s="5"/>
+      <c r="AW20" s="5"/>
+      <c r="AX20" s="5"/>
+      <c r="AY20" s="5"/>
+      <c r="AZ20" s="5"/>
+      <c r="BA20" s="5"/>
+      <c r="BB20" s="5"/>
+      <c r="BC20" s="5"/>
+      <c r="BD20" s="5"/>
+      <c r="BE20" s="28"/>
+      <c r="BF20" s="27"/>
+    </row>
+    <row r="21" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="4" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C21" s="6">
         <v>103</v>
@@ -1757,7 +2438,7 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L21" s="6">
         <v>1</v>
@@ -1778,14 +2459,43 @@
       <c r="Z21" s="6"/>
       <c r="AA21" s="6"/>
       <c r="AB21" s="6"/>
-      <c r="AC21" s="3"/>
-      <c r="AD21" s="3"/>
+      <c r="AC21" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD21" s="7"/>
       <c r="AE21" s="3"/>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF21" s="28"/>
+      <c r="AG21" s="5"/>
+      <c r="AH21" s="5"/>
+      <c r="AI21" s="5"/>
+      <c r="AJ21" s="5"/>
+      <c r="AK21" s="5"/>
+      <c r="AL21" s="5"/>
+      <c r="AM21" s="5"/>
+      <c r="AN21" s="5"/>
+      <c r="AO21" s="5"/>
+      <c r="AP21" s="5"/>
+      <c r="AQ21" s="5"/>
+      <c r="AR21" s="5"/>
+      <c r="AS21" s="5"/>
+      <c r="AT21" s="5"/>
+      <c r="AU21" s="5"/>
+      <c r="AV21" s="5"/>
+      <c r="AW21" s="5"/>
+      <c r="AX21" s="5"/>
+      <c r="AY21" s="5"/>
+      <c r="AZ21" s="5"/>
+      <c r="BA21" s="5"/>
+      <c r="BB21" s="5"/>
+      <c r="BC21" s="5"/>
+      <c r="BD21" s="5"/>
+      <c r="BE21" s="28"/>
+      <c r="BF21" s="27"/>
+    </row>
+    <row r="22" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="4" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C22" s="6">
         <v>103</v>
@@ -1821,14 +2531,43 @@
       <c r="Z22" s="6"/>
       <c r="AA22" s="6"/>
       <c r="AB22" s="6"/>
-      <c r="AC22" s="3"/>
-      <c r="AD22" s="3"/>
+      <c r="AC22" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="7"/>
       <c r="AE22" s="3"/>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF22" s="28"/>
+      <c r="AG22" s="5"/>
+      <c r="AH22" s="5"/>
+      <c r="AI22" s="5"/>
+      <c r="AJ22" s="5"/>
+      <c r="AK22" s="5"/>
+      <c r="AL22" s="5"/>
+      <c r="AM22" s="5"/>
+      <c r="AN22" s="5"/>
+      <c r="AO22" s="5"/>
+      <c r="AP22" s="5"/>
+      <c r="AQ22" s="5"/>
+      <c r="AR22" s="5"/>
+      <c r="AS22" s="5"/>
+      <c r="AT22" s="5"/>
+      <c r="AU22" s="5"/>
+      <c r="AV22" s="5"/>
+      <c r="AW22" s="5"/>
+      <c r="AX22" s="5"/>
+      <c r="AY22" s="5"/>
+      <c r="AZ22" s="5"/>
+      <c r="BA22" s="5"/>
+      <c r="BB22" s="5"/>
+      <c r="BC22" s="5"/>
+      <c r="BD22" s="5"/>
+      <c r="BE22" s="28"/>
+      <c r="BF22" s="27"/>
+    </row>
+    <row r="23" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="4" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C23" s="6">
         <v>103</v>
@@ -1864,23 +2603,52 @@
       <c r="Z23" s="6"/>
       <c r="AA23" s="6"/>
       <c r="AB23" s="6"/>
-      <c r="AC23" s="3"/>
-      <c r="AD23" s="3"/>
+      <c r="AC23" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD23" s="7"/>
       <c r="AE23" s="3"/>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF23" s="28"/>
+      <c r="AG23" s="5"/>
+      <c r="AH23" s="5"/>
+      <c r="AI23" s="5"/>
+      <c r="AJ23" s="5"/>
+      <c r="AK23" s="5"/>
+      <c r="AL23" s="5"/>
+      <c r="AM23" s="5"/>
+      <c r="AN23" s="5"/>
+      <c r="AO23" s="5"/>
+      <c r="AP23" s="5"/>
+      <c r="AQ23" s="5"/>
+      <c r="AR23" s="5"/>
+      <c r="AS23" s="5"/>
+      <c r="AT23" s="5"/>
+      <c r="AU23" s="5"/>
+      <c r="AV23" s="5"/>
+      <c r="AW23" s="5"/>
+      <c r="AX23" s="5"/>
+      <c r="AY23" s="5"/>
+      <c r="AZ23" s="5"/>
+      <c r="BA23" s="5"/>
+      <c r="BB23" s="5"/>
+      <c r="BC23" s="5"/>
+      <c r="BD23" s="5"/>
+      <c r="BE23" s="28"/>
+      <c r="BF23" s="27"/>
+    </row>
+    <row r="24" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C24" s="6">
         <v>103</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>18</v>
+      <c r="D24" s="20" t="s">
+        <v>17</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -1888,10 +2656,10 @@
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
@@ -1909,14 +2677,45 @@
       <c r="Z24" s="6"/>
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
-      <c r="AC24" s="3"/>
-      <c r="AD24" s="3"/>
+      <c r="AC24" s="20">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="AE24" s="3"/>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF24" s="28"/>
+      <c r="AG24" s="5"/>
+      <c r="AH24" s="5"/>
+      <c r="AI24" s="5"/>
+      <c r="AJ24" s="5"/>
+      <c r="AK24" s="5"/>
+      <c r="AL24" s="5"/>
+      <c r="AM24" s="5"/>
+      <c r="AN24" s="5"/>
+      <c r="AO24" s="5"/>
+      <c r="AP24" s="5"/>
+      <c r="AQ24" s="5"/>
+      <c r="AR24" s="5"/>
+      <c r="AS24" s="5"/>
+      <c r="AT24" s="5"/>
+      <c r="AU24" s="5"/>
+      <c r="AV24" s="5"/>
+      <c r="AW24" s="5"/>
+      <c r="AX24" s="5"/>
+      <c r="AY24" s="5"/>
+      <c r="AZ24" s="5"/>
+      <c r="BA24" s="5"/>
+      <c r="BB24" s="5"/>
+      <c r="BC24" s="5"/>
+      <c r="BD24" s="5"/>
+      <c r="BE24" s="28"/>
+      <c r="BF24" s="27"/>
+    </row>
+    <row r="25" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="4" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C25" s="6">
         <v>104</v>
@@ -1954,14 +2753,43 @@
       <c r="Z25" s="6"/>
       <c r="AA25" s="6"/>
       <c r="AB25" s="6"/>
-      <c r="AC25" s="3"/>
-      <c r="AD25" s="3"/>
+      <c r="AC25" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD25" s="7"/>
       <c r="AE25" s="3"/>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF25" s="28"/>
+      <c r="AG25" s="5"/>
+      <c r="AH25" s="5"/>
+      <c r="AI25" s="5"/>
+      <c r="AJ25" s="5"/>
+      <c r="AK25" s="5"/>
+      <c r="AL25" s="5"/>
+      <c r="AM25" s="5"/>
+      <c r="AN25" s="5"/>
+      <c r="AO25" s="5"/>
+      <c r="AP25" s="5"/>
+      <c r="AQ25" s="5"/>
+      <c r="AR25" s="5"/>
+      <c r="AS25" s="5"/>
+      <c r="AT25" s="5"/>
+      <c r="AU25" s="5"/>
+      <c r="AV25" s="5"/>
+      <c r="AW25" s="5"/>
+      <c r="AX25" s="5"/>
+      <c r="AY25" s="5"/>
+      <c r="AZ25" s="5"/>
+      <c r="BA25" s="5"/>
+      <c r="BB25" s="5"/>
+      <c r="BC25" s="5"/>
+      <c r="BD25" s="5"/>
+      <c r="BE25" s="28"/>
+      <c r="BF25" s="27"/>
+    </row>
+    <row r="26" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="4" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C26" s="6">
         <v>104</v>
@@ -1999,14 +2827,43 @@
       <c r="Z26" s="6"/>
       <c r="AA26" s="6"/>
       <c r="AB26" s="6"/>
-      <c r="AC26" s="3"/>
-      <c r="AD26" s="3"/>
+      <c r="AC26" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="7"/>
       <c r="AE26" s="3"/>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF26" s="28"/>
+      <c r="AG26" s="5"/>
+      <c r="AH26" s="5"/>
+      <c r="AI26" s="5"/>
+      <c r="AJ26" s="5"/>
+      <c r="AK26" s="5"/>
+      <c r="AL26" s="5"/>
+      <c r="AM26" s="5"/>
+      <c r="AN26" s="5"/>
+      <c r="AO26" s="5"/>
+      <c r="AP26" s="5"/>
+      <c r="AQ26" s="5"/>
+      <c r="AR26" s="5"/>
+      <c r="AS26" s="5"/>
+      <c r="AT26" s="5"/>
+      <c r="AU26" s="5"/>
+      <c r="AV26" s="5"/>
+      <c r="AW26" s="5"/>
+      <c r="AX26" s="5"/>
+      <c r="AY26" s="5"/>
+      <c r="AZ26" s="5"/>
+      <c r="BA26" s="5"/>
+      <c r="BB26" s="5"/>
+      <c r="BC26" s="5"/>
+      <c r="BD26" s="5"/>
+      <c r="BE26" s="28"/>
+      <c r="BF26" s="27"/>
+    </row>
+    <row r="27" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="4" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C27" s="6">
         <v>104</v>
@@ -2044,14 +2901,43 @@
       <c r="Z27" s="6"/>
       <c r="AA27" s="6"/>
       <c r="AB27" s="6"/>
-      <c r="AC27" s="3"/>
-      <c r="AD27" s="3"/>
+      <c r="AC27" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD27" s="7"/>
       <c r="AE27" s="3"/>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF27" s="28"/>
+      <c r="AG27" s="5"/>
+      <c r="AH27" s="5"/>
+      <c r="AI27" s="5"/>
+      <c r="AJ27" s="5"/>
+      <c r="AK27" s="5"/>
+      <c r="AL27" s="5"/>
+      <c r="AM27" s="5"/>
+      <c r="AN27" s="5"/>
+      <c r="AO27" s="5"/>
+      <c r="AP27" s="5"/>
+      <c r="AQ27" s="5"/>
+      <c r="AR27" s="5"/>
+      <c r="AS27" s="5"/>
+      <c r="AT27" s="5"/>
+      <c r="AU27" s="5"/>
+      <c r="AV27" s="5"/>
+      <c r="AW27" s="5"/>
+      <c r="AX27" s="5"/>
+      <c r="AY27" s="5"/>
+      <c r="AZ27" s="5"/>
+      <c r="BA27" s="5"/>
+      <c r="BB27" s="5"/>
+      <c r="BC27" s="5"/>
+      <c r="BD27" s="5"/>
+      <c r="BE27" s="28"/>
+      <c r="BF27" s="27"/>
+    </row>
+    <row r="28" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C28" s="6">
         <v>104</v>
@@ -2089,14 +2975,43 @@
       <c r="Z28" s="6"/>
       <c r="AA28" s="6"/>
       <c r="AB28" s="6"/>
-      <c r="AC28" s="3"/>
-      <c r="AD28" s="3"/>
+      <c r="AC28" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD28" s="7"/>
       <c r="AE28" s="3"/>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF28" s="28"/>
+      <c r="AG28" s="5"/>
+      <c r="AH28" s="5"/>
+      <c r="AI28" s="5"/>
+      <c r="AJ28" s="5"/>
+      <c r="AK28" s="5"/>
+      <c r="AL28" s="5"/>
+      <c r="AM28" s="5"/>
+      <c r="AN28" s="5"/>
+      <c r="AO28" s="5"/>
+      <c r="AP28" s="5"/>
+      <c r="AQ28" s="5"/>
+      <c r="AR28" s="5"/>
+      <c r="AS28" s="5"/>
+      <c r="AT28" s="5"/>
+      <c r="AU28" s="5"/>
+      <c r="AV28" s="5"/>
+      <c r="AW28" s="5"/>
+      <c r="AX28" s="5"/>
+      <c r="AY28" s="5"/>
+      <c r="AZ28" s="5"/>
+      <c r="BA28" s="5"/>
+      <c r="BB28" s="5"/>
+      <c r="BC28" s="5"/>
+      <c r="BD28" s="5"/>
+      <c r="BE28" s="28"/>
+      <c r="BF28" s="27"/>
+    </row>
+    <row r="29" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="4" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C29" s="6">
         <v>104</v>
@@ -2134,14 +3049,43 @@
       <c r="Z29" s="6"/>
       <c r="AA29" s="6"/>
       <c r="AB29" s="6"/>
-      <c r="AC29" s="3"/>
-      <c r="AD29" s="3"/>
+      <c r="AC29" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD29" s="7"/>
       <c r="AE29" s="3"/>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF29" s="28"/>
+      <c r="AG29" s="5"/>
+      <c r="AH29" s="5"/>
+      <c r="AI29" s="5"/>
+      <c r="AJ29" s="5"/>
+      <c r="AK29" s="5"/>
+      <c r="AL29" s="5"/>
+      <c r="AM29" s="5"/>
+      <c r="AN29" s="5"/>
+      <c r="AO29" s="5"/>
+      <c r="AP29" s="5"/>
+      <c r="AQ29" s="5"/>
+      <c r="AR29" s="5"/>
+      <c r="AS29" s="5"/>
+      <c r="AT29" s="5"/>
+      <c r="AU29" s="5"/>
+      <c r="AV29" s="5"/>
+      <c r="AW29" s="5"/>
+      <c r="AX29" s="5"/>
+      <c r="AY29" s="5"/>
+      <c r="AZ29" s="5"/>
+      <c r="BA29" s="5"/>
+      <c r="BB29" s="5"/>
+      <c r="BC29" s="5"/>
+      <c r="BD29" s="5"/>
+      <c r="BE29" s="28"/>
+      <c r="BF29" s="27"/>
+    </row>
+    <row r="30" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="4" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C30" s="6">
         <v>104</v>
@@ -2158,10 +3102,10 @@
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
       <c r="M30" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O30" s="6">
         <v>1</v>
@@ -2179,23 +3123,52 @@
       <c r="Z30" s="6"/>
       <c r="AA30" s="6"/>
       <c r="AB30" s="6"/>
-      <c r="AC30" s="3"/>
-      <c r="AD30" s="3"/>
+      <c r="AC30" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD30" s="7"/>
       <c r="AE30" s="3"/>
-    </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF30" s="28"/>
+      <c r="AG30" s="5"/>
+      <c r="AH30" s="5"/>
+      <c r="AI30" s="5"/>
+      <c r="AJ30" s="5"/>
+      <c r="AK30" s="5"/>
+      <c r="AL30" s="5"/>
+      <c r="AM30" s="5"/>
+      <c r="AN30" s="5"/>
+      <c r="AO30" s="5"/>
+      <c r="AP30" s="5"/>
+      <c r="AQ30" s="5"/>
+      <c r="AR30" s="5"/>
+      <c r="AS30" s="5"/>
+      <c r="AT30" s="5"/>
+      <c r="AU30" s="5"/>
+      <c r="AV30" s="5"/>
+      <c r="AW30" s="5"/>
+      <c r="AX30" s="5"/>
+      <c r="AY30" s="5"/>
+      <c r="AZ30" s="5"/>
+      <c r="BA30" s="5"/>
+      <c r="BB30" s="5"/>
+      <c r="BC30" s="5"/>
+      <c r="BD30" s="5"/>
+      <c r="BE30" s="28"/>
+      <c r="BF30" s="27"/>
+    </row>
+    <row r="31" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="4" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C31" s="6">
         <v>104</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>18</v>
+      <c r="D31" s="20" t="s">
+        <v>17</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
@@ -2205,13 +3178,13 @@
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O31" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
@@ -2226,13 +3199,44 @@
       <c r="Z31" s="6"/>
       <c r="AA31" s="6"/>
       <c r="AB31" s="6"/>
-      <c r="AC31" s="3"/>
-      <c r="AD31" s="3"/>
+      <c r="AC31" s="20">
+        <v>0</v>
+      </c>
+      <c r="AD31" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="AE31" s="3"/>
-    </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF31" s="28"/>
+      <c r="AG31" s="5"/>
+      <c r="AH31" s="5"/>
+      <c r="AI31" s="5"/>
+      <c r="AJ31" s="5"/>
+      <c r="AK31" s="5"/>
+      <c r="AL31" s="5"/>
+      <c r="AM31" s="5"/>
+      <c r="AN31" s="5"/>
+      <c r="AO31" s="5"/>
+      <c r="AP31" s="5"/>
+      <c r="AQ31" s="5"/>
+      <c r="AR31" s="5"/>
+      <c r="AS31" s="5"/>
+      <c r="AT31" s="5"/>
+      <c r="AU31" s="5"/>
+      <c r="AV31" s="5"/>
+      <c r="AW31" s="5"/>
+      <c r="AX31" s="5"/>
+      <c r="AY31" s="5"/>
+      <c r="AZ31" s="5"/>
+      <c r="BA31" s="5"/>
+      <c r="BB31" s="5"/>
+      <c r="BC31" s="5"/>
+      <c r="BD31" s="5"/>
+      <c r="BE31" s="28"/>
+      <c r="BF31" s="27"/>
+    </row>
+    <row r="32" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C32" s="6">
         <v>106</v>
@@ -2267,13 +3271,42 @@
       <c r="Z32" s="6"/>
       <c r="AA32" s="6"/>
       <c r="AB32" s="6"/>
-      <c r="AC32" s="3"/>
-      <c r="AD32" s="3"/>
+      <c r="AC32" s="6">
+        <v>4</v>
+      </c>
+      <c r="AD32" s="6"/>
       <c r="AE32" s="3"/>
-    </row>
-    <row r="33" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF32" s="28"/>
+      <c r="AG32" s="5"/>
+      <c r="AH32" s="5"/>
+      <c r="AI32" s="5"/>
+      <c r="AJ32" s="5"/>
+      <c r="AK32" s="5"/>
+      <c r="AL32" s="5"/>
+      <c r="AM32" s="5"/>
+      <c r="AN32" s="5"/>
+      <c r="AO32" s="5"/>
+      <c r="AP32" s="5"/>
+      <c r="AQ32" s="5"/>
+      <c r="AR32" s="5"/>
+      <c r="AS32" s="5"/>
+      <c r="AT32" s="5"/>
+      <c r="AU32" s="5"/>
+      <c r="AV32" s="5"/>
+      <c r="AW32" s="5"/>
+      <c r="AX32" s="5"/>
+      <c r="AY32" s="5"/>
+      <c r="AZ32" s="5"/>
+      <c r="BA32" s="5"/>
+      <c r="BB32" s="5"/>
+      <c r="BC32" s="5"/>
+      <c r="BD32" s="5"/>
+      <c r="BE32" s="28"/>
+      <c r="BF32" s="27"/>
+    </row>
+    <row r="33" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C33" s="6">
         <v>106</v>
@@ -2283,7 +3316,7 @@
         <v>missing</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
@@ -2296,7 +3329,7 @@
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
       <c r="P33" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
@@ -2310,23 +3343,54 @@
       <c r="Z33" s="6"/>
       <c r="AA33" s="6"/>
       <c r="AB33" s="6"/>
-      <c r="AC33" s="3"/>
-      <c r="AD33" s="3"/>
+      <c r="AC33" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD33" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="AE33" s="3"/>
-    </row>
-    <row r="34" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF33" s="28"/>
+      <c r="AG33" s="5"/>
+      <c r="AH33" s="5"/>
+      <c r="AI33" s="5"/>
+      <c r="AJ33" s="5"/>
+      <c r="AK33" s="5"/>
+      <c r="AL33" s="5"/>
+      <c r="AM33" s="5"/>
+      <c r="AN33" s="5"/>
+      <c r="AO33" s="5"/>
+      <c r="AP33" s="5"/>
+      <c r="AQ33" s="5"/>
+      <c r="AR33" s="5"/>
+      <c r="AS33" s="5"/>
+      <c r="AT33" s="5"/>
+      <c r="AU33" s="5"/>
+      <c r="AV33" s="5"/>
+      <c r="AW33" s="5"/>
+      <c r="AX33" s="5"/>
+      <c r="AY33" s="5"/>
+      <c r="AZ33" s="5"/>
+      <c r="BA33" s="5"/>
+      <c r="BB33" s="5"/>
+      <c r="BC33" s="5"/>
+      <c r="BD33" s="5"/>
+      <c r="BE33" s="28"/>
+      <c r="BF33" s="27"/>
+    </row>
+    <row r="34" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C34" s="6">
         <v>106</v>
       </c>
-      <c r="D34" s="6" t="str">
+      <c r="D34" s="22" t="str">
         <f>IF(OR(P34= "-",P34&lt;0), "missing", P34)</f>
         <v>missing</v>
       </c>
-      <c r="E34" s="9" t="s">
-        <v>21</v>
+      <c r="E34" s="23" t="s">
+        <v>20</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
@@ -2353,13 +3417,44 @@
       <c r="Z34" s="6"/>
       <c r="AA34" s="6"/>
       <c r="AB34" s="6"/>
-      <c r="AC34" s="3"/>
-      <c r="AD34" s="3"/>
+      <c r="AC34" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD34" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="AE34" s="3"/>
-    </row>
-    <row r="35" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF34" s="28"/>
+      <c r="AG34" s="5"/>
+      <c r="AH34" s="5"/>
+      <c r="AI34" s="5"/>
+      <c r="AJ34" s="5"/>
+      <c r="AK34" s="5"/>
+      <c r="AL34" s="5"/>
+      <c r="AM34" s="5"/>
+      <c r="AN34" s="5"/>
+      <c r="AO34" s="5"/>
+      <c r="AP34" s="5"/>
+      <c r="AQ34" s="5"/>
+      <c r="AR34" s="5"/>
+      <c r="AS34" s="5"/>
+      <c r="AT34" s="5"/>
+      <c r="AU34" s="5"/>
+      <c r="AV34" s="5"/>
+      <c r="AW34" s="5"/>
+      <c r="AX34" s="5"/>
+      <c r="AY34" s="5"/>
+      <c r="AZ34" s="5"/>
+      <c r="BA34" s="5"/>
+      <c r="BB34" s="5"/>
+      <c r="BC34" s="5"/>
+      <c r="BD34" s="5"/>
+      <c r="BE34" s="28"/>
+      <c r="BF34" s="27"/>
+    </row>
+    <row r="35" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C35" s="6">
         <v>107</v>
@@ -2393,13 +3488,42 @@
       <c r="Z35" s="6"/>
       <c r="AA35" s="6"/>
       <c r="AB35" s="6"/>
-      <c r="AC35" s="3"/>
-      <c r="AD35" s="3"/>
+      <c r="AC35" s="6">
+        <v>5</v>
+      </c>
+      <c r="AD35" s="6"/>
       <c r="AE35" s="3"/>
-    </row>
-    <row r="36" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF35" s="28"/>
+      <c r="AG35" s="5"/>
+      <c r="AH35" s="5"/>
+      <c r="AI35" s="5"/>
+      <c r="AJ35" s="5"/>
+      <c r="AK35" s="5"/>
+      <c r="AL35" s="5"/>
+      <c r="AM35" s="5"/>
+      <c r="AN35" s="5"/>
+      <c r="AO35" s="5"/>
+      <c r="AP35" s="5"/>
+      <c r="AQ35" s="5"/>
+      <c r="AR35" s="5"/>
+      <c r="AS35" s="5"/>
+      <c r="AT35" s="5"/>
+      <c r="AU35" s="5"/>
+      <c r="AV35" s="5"/>
+      <c r="AW35" s="5"/>
+      <c r="AX35" s="5"/>
+      <c r="AY35" s="5"/>
+      <c r="AZ35" s="5"/>
+      <c r="BA35" s="5"/>
+      <c r="BB35" s="5"/>
+      <c r="BC35" s="5"/>
+      <c r="BD35" s="5"/>
+      <c r="BE35" s="28"/>
+      <c r="BF35" s="27"/>
+    </row>
+    <row r="36" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C36" s="6">
         <v>107</v>
@@ -2409,7 +3533,7 @@
         <v>missing</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
@@ -2423,7 +3547,7 @@
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
       <c r="Q36" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R36" s="6"/>
       <c r="S36" s="6"/>
@@ -2436,13 +3560,44 @@
       <c r="Z36" s="6"/>
       <c r="AA36" s="6"/>
       <c r="AB36" s="6"/>
-      <c r="AC36" s="3"/>
-      <c r="AD36" s="3"/>
+      <c r="AC36" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD36" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="AE36" s="3"/>
-    </row>
-    <row r="37" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF36" s="28"/>
+      <c r="AG36" s="5"/>
+      <c r="AH36" s="5"/>
+      <c r="AI36" s="5"/>
+      <c r="AJ36" s="5"/>
+      <c r="AK36" s="5"/>
+      <c r="AL36" s="5"/>
+      <c r="AM36" s="5"/>
+      <c r="AN36" s="5"/>
+      <c r="AO36" s="5"/>
+      <c r="AP36" s="5"/>
+      <c r="AQ36" s="5"/>
+      <c r="AR36" s="5"/>
+      <c r="AS36" s="5"/>
+      <c r="AT36" s="5"/>
+      <c r="AU36" s="5"/>
+      <c r="AV36" s="5"/>
+      <c r="AW36" s="5"/>
+      <c r="AX36" s="5"/>
+      <c r="AY36" s="5"/>
+      <c r="AZ36" s="5"/>
+      <c r="BA36" s="5"/>
+      <c r="BB36" s="5"/>
+      <c r="BC36" s="5"/>
+      <c r="BD36" s="5"/>
+      <c r="BE36" s="28"/>
+      <c r="BF36" s="27"/>
+    </row>
+    <row r="37" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C37" s="6">
         <v>107</v>
@@ -2452,7 +3607,7 @@
         <v>missing</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -2479,13 +3634,44 @@
       <c r="Z37" s="6"/>
       <c r="AA37" s="6"/>
       <c r="AB37" s="6"/>
-      <c r="AC37" s="3"/>
-      <c r="AD37" s="3"/>
+      <c r="AC37" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD37" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="AE37" s="3"/>
-    </row>
-    <row r="38" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF37" s="28"/>
+      <c r="AG37" s="5"/>
+      <c r="AH37" s="5"/>
+      <c r="AI37" s="5"/>
+      <c r="AJ37" s="5"/>
+      <c r="AK37" s="5"/>
+      <c r="AL37" s="5"/>
+      <c r="AM37" s="5"/>
+      <c r="AN37" s="5"/>
+      <c r="AO37" s="5"/>
+      <c r="AP37" s="5"/>
+      <c r="AQ37" s="5"/>
+      <c r="AR37" s="5"/>
+      <c r="AS37" s="5"/>
+      <c r="AT37" s="5"/>
+      <c r="AU37" s="5"/>
+      <c r="AV37" s="5"/>
+      <c r="AW37" s="5"/>
+      <c r="AX37" s="5"/>
+      <c r="AY37" s="5"/>
+      <c r="AZ37" s="5"/>
+      <c r="BA37" s="5"/>
+      <c r="BB37" s="5"/>
+      <c r="BC37" s="5"/>
+      <c r="BD37" s="5"/>
+      <c r="BE37" s="28"/>
+      <c r="BF37" s="27"/>
+    </row>
+    <row r="38" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C38" s="6">
         <v>108</v>
@@ -2519,22 +3705,51 @@
       <c r="Z38" s="6"/>
       <c r="AA38" s="6"/>
       <c r="AB38" s="6"/>
-      <c r="AC38" s="3"/>
-      <c r="AD38" s="3"/>
+      <c r="AC38" s="6">
+        <v>500</v>
+      </c>
+      <c r="AD38" s="6"/>
       <c r="AE38" s="3"/>
-    </row>
-    <row r="39" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF38" s="28"/>
+      <c r="AG38" s="5"/>
+      <c r="AH38" s="5"/>
+      <c r="AI38" s="5"/>
+      <c r="AJ38" s="5"/>
+      <c r="AK38" s="5"/>
+      <c r="AL38" s="5"/>
+      <c r="AM38" s="5"/>
+      <c r="AN38" s="5"/>
+      <c r="AO38" s="5"/>
+      <c r="AP38" s="5"/>
+      <c r="AQ38" s="5"/>
+      <c r="AR38" s="5"/>
+      <c r="AS38" s="5"/>
+      <c r="AT38" s="5"/>
+      <c r="AU38" s="5"/>
+      <c r="AV38" s="5"/>
+      <c r="AW38" s="5"/>
+      <c r="AX38" s="5"/>
+      <c r="AY38" s="5"/>
+      <c r="AZ38" s="5"/>
+      <c r="BA38" s="5"/>
+      <c r="BB38" s="5"/>
+      <c r="BC38" s="5"/>
+      <c r="BD38" s="5"/>
+      <c r="BE38" s="28"/>
+      <c r="BF38" s="27"/>
+    </row>
+    <row r="39" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C39" s="6">
         <v>108</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
@@ -2549,7 +3764,7 @@
       <c r="P39" s="6"/>
       <c r="Q39" s="6"/>
       <c r="R39" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S39" s="6"/>
       <c r="T39" s="6"/>
@@ -2561,13 +3776,44 @@
       <c r="Z39" s="6"/>
       <c r="AA39" s="6"/>
       <c r="AB39" s="6"/>
-      <c r="AC39" s="3"/>
-      <c r="AD39" s="3"/>
+      <c r="AC39" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD39" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="AE39" s="3"/>
-    </row>
-    <row r="40" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF39" s="28"/>
+      <c r="AG39" s="5"/>
+      <c r="AH39" s="5"/>
+      <c r="AI39" s="5"/>
+      <c r="AJ39" s="5"/>
+      <c r="AK39" s="5"/>
+      <c r="AL39" s="5"/>
+      <c r="AM39" s="5"/>
+      <c r="AN39" s="5"/>
+      <c r="AO39" s="5"/>
+      <c r="AP39" s="5"/>
+      <c r="AQ39" s="5"/>
+      <c r="AR39" s="5"/>
+      <c r="AS39" s="5"/>
+      <c r="AT39" s="5"/>
+      <c r="AU39" s="5"/>
+      <c r="AV39" s="5"/>
+      <c r="AW39" s="5"/>
+      <c r="AX39" s="5"/>
+      <c r="AY39" s="5"/>
+      <c r="AZ39" s="5"/>
+      <c r="BA39" s="5"/>
+      <c r="BB39" s="5"/>
+      <c r="BC39" s="5"/>
+      <c r="BD39" s="5"/>
+      <c r="BE39" s="28"/>
+      <c r="BF39" s="27"/>
+    </row>
+    <row r="40" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C40" s="6">
         <v>108</v>
@@ -2577,7 +3823,7 @@
         <v>missing</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
@@ -2604,13 +3850,44 @@
       <c r="Z40" s="6"/>
       <c r="AA40" s="6"/>
       <c r="AB40" s="6"/>
-      <c r="AC40" s="3"/>
-      <c r="AD40" s="3"/>
+      <c r="AC40" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD40" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="AE40" s="3"/>
-    </row>
-    <row r="41" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF40" s="28"/>
+      <c r="AG40" s="5"/>
+      <c r="AH40" s="5"/>
+      <c r="AI40" s="5"/>
+      <c r="AJ40" s="5"/>
+      <c r="AK40" s="5"/>
+      <c r="AL40" s="5"/>
+      <c r="AM40" s="5"/>
+      <c r="AN40" s="5"/>
+      <c r="AO40" s="5"/>
+      <c r="AP40" s="5"/>
+      <c r="AQ40" s="5"/>
+      <c r="AR40" s="5"/>
+      <c r="AS40" s="5"/>
+      <c r="AT40" s="5"/>
+      <c r="AU40" s="5"/>
+      <c r="AV40" s="5"/>
+      <c r="AW40" s="5"/>
+      <c r="AX40" s="5"/>
+      <c r="AY40" s="5"/>
+      <c r="AZ40" s="5"/>
+      <c r="BA40" s="5"/>
+      <c r="BB40" s="5"/>
+      <c r="BC40" s="5"/>
+      <c r="BD40" s="5"/>
+      <c r="BE40" s="28"/>
+      <c r="BF40" s="27"/>
+    </row>
+    <row r="41" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C41" s="6">
         <v>109</v>
@@ -2645,13 +3922,42 @@
       <c r="Z41" s="6"/>
       <c r="AA41" s="6"/>
       <c r="AB41" s="6"/>
-      <c r="AC41" s="3"/>
+      <c r="AC41" s="24" t="s">
+        <v>113</v>
+      </c>
       <c r="AD41" s="3"/>
       <c r="AE41" s="3"/>
-    </row>
-    <row r="42" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF41" s="28"/>
+      <c r="AG41" s="5"/>
+      <c r="AH41" s="5"/>
+      <c r="AI41" s="5"/>
+      <c r="AJ41" s="5"/>
+      <c r="AK41" s="5"/>
+      <c r="AL41" s="5"/>
+      <c r="AM41" s="5"/>
+      <c r="AN41" s="5"/>
+      <c r="AO41" s="5"/>
+      <c r="AP41" s="5"/>
+      <c r="AQ41" s="5"/>
+      <c r="AR41" s="5"/>
+      <c r="AS41" s="5"/>
+      <c r="AT41" s="5"/>
+      <c r="AU41" s="5"/>
+      <c r="AV41" s="5"/>
+      <c r="AW41" s="5"/>
+      <c r="AX41" s="5"/>
+      <c r="AY41" s="5"/>
+      <c r="AZ41" s="5"/>
+      <c r="BA41" s="5"/>
+      <c r="BB41" s="5"/>
+      <c r="BC41" s="5"/>
+      <c r="BD41" s="5"/>
+      <c r="BE41" s="28"/>
+      <c r="BF41" s="27"/>
+    </row>
+    <row r="42" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C42" s="6">
         <v>109</v>
@@ -2661,7 +3967,7 @@
         <v>missing</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
@@ -2677,7 +3983,7 @@
       <c r="Q42" s="6"/>
       <c r="R42" s="6"/>
       <c r="S42" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T42" s="6"/>
       <c r="U42" s="6"/>
@@ -2688,13 +3994,44 @@
       <c r="Z42" s="6"/>
       <c r="AA42" s="6"/>
       <c r="AB42" s="6"/>
-      <c r="AC42" s="3"/>
-      <c r="AD42" s="3"/>
+      <c r="AC42" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD42" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="AE42" s="3"/>
-    </row>
-    <row r="43" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF42" s="28"/>
+      <c r="AG42" s="5"/>
+      <c r="AH42" s="5"/>
+      <c r="AI42" s="5"/>
+      <c r="AJ42" s="5"/>
+      <c r="AK42" s="5"/>
+      <c r="AL42" s="5"/>
+      <c r="AM42" s="5"/>
+      <c r="AN42" s="5"/>
+      <c r="AO42" s="5"/>
+      <c r="AP42" s="5"/>
+      <c r="AQ42" s="5"/>
+      <c r="AR42" s="5"/>
+      <c r="AS42" s="5"/>
+      <c r="AT42" s="5"/>
+      <c r="AU42" s="5"/>
+      <c r="AV42" s="5"/>
+      <c r="AW42" s="5"/>
+      <c r="AX42" s="5"/>
+      <c r="AY42" s="5"/>
+      <c r="AZ42" s="5"/>
+      <c r="BA42" s="5"/>
+      <c r="BB42" s="5"/>
+      <c r="BC42" s="5"/>
+      <c r="BD42" s="5"/>
+      <c r="BE42" s="28"/>
+      <c r="BF42" s="27"/>
+    </row>
+    <row r="43" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C43" s="6">
         <v>109</v>
@@ -2704,7 +4041,7 @@
         <v>missing</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
@@ -2731,13 +4068,44 @@
       <c r="Z43" s="6"/>
       <c r="AA43" s="6"/>
       <c r="AB43" s="6"/>
-      <c r="AC43" s="3"/>
-      <c r="AD43" s="3"/>
+      <c r="AC43" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD43" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="AE43" s="3"/>
-    </row>
-    <row r="44" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF43" s="28"/>
+      <c r="AG43" s="5"/>
+      <c r="AH43" s="5"/>
+      <c r="AI43" s="5"/>
+      <c r="AJ43" s="5"/>
+      <c r="AK43" s="5"/>
+      <c r="AL43" s="5"/>
+      <c r="AM43" s="5"/>
+      <c r="AN43" s="5"/>
+      <c r="AO43" s="5"/>
+      <c r="AP43" s="5"/>
+      <c r="AQ43" s="5"/>
+      <c r="AR43" s="5"/>
+      <c r="AS43" s="5"/>
+      <c r="AT43" s="5"/>
+      <c r="AU43" s="5"/>
+      <c r="AV43" s="5"/>
+      <c r="AW43" s="5"/>
+      <c r="AX43" s="5"/>
+      <c r="AY43" s="5"/>
+      <c r="AZ43" s="5"/>
+      <c r="BA43" s="5"/>
+      <c r="BB43" s="5"/>
+      <c r="BC43" s="5"/>
+      <c r="BD43" s="5"/>
+      <c r="BE43" s="28"/>
+      <c r="BF43" s="27"/>
+    </row>
+    <row r="44" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C44" s="6">
         <v>110</v>
@@ -2772,13 +4140,42 @@
       <c r="Z44" s="6"/>
       <c r="AA44" s="6"/>
       <c r="AB44" s="6"/>
-      <c r="AC44" s="3"/>
+      <c r="AC44" s="24" t="s">
+        <v>114</v>
+      </c>
       <c r="AD44" s="3"/>
       <c r="AE44" s="3"/>
-    </row>
-    <row r="45" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF44" s="28"/>
+      <c r="AG44" s="5"/>
+      <c r="AH44" s="5"/>
+      <c r="AI44" s="5"/>
+      <c r="AJ44" s="5"/>
+      <c r="AK44" s="5"/>
+      <c r="AL44" s="5"/>
+      <c r="AM44" s="5"/>
+      <c r="AN44" s="5"/>
+      <c r="AO44" s="5"/>
+      <c r="AP44" s="5"/>
+      <c r="AQ44" s="5"/>
+      <c r="AR44" s="5"/>
+      <c r="AS44" s="5"/>
+      <c r="AT44" s="5"/>
+      <c r="AU44" s="5"/>
+      <c r="AV44" s="5"/>
+      <c r="AW44" s="5"/>
+      <c r="AX44" s="5"/>
+      <c r="AY44" s="5"/>
+      <c r="AZ44" s="5"/>
+      <c r="BA44" s="5"/>
+      <c r="BB44" s="5"/>
+      <c r="BC44" s="5"/>
+      <c r="BD44" s="5"/>
+      <c r="BE44" s="28"/>
+      <c r="BF44" s="27"/>
+    </row>
+    <row r="45" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C45" s="6">
         <v>110</v>
@@ -2788,7 +4185,7 @@
         <v>missing</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
@@ -2805,7 +4202,7 @@
       <c r="R45" s="6"/>
       <c r="S45" s="6"/>
       <c r="T45" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U45" s="6"/>
       <c r="V45" s="6"/>
@@ -2815,13 +4212,44 @@
       <c r="Z45" s="6"/>
       <c r="AA45" s="6"/>
       <c r="AB45" s="6"/>
-      <c r="AC45" s="3"/>
-      <c r="AD45" s="3"/>
+      <c r="AC45" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD45" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="AE45" s="3"/>
-    </row>
-    <row r="46" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF45" s="28"/>
+      <c r="AG45" s="5"/>
+      <c r="AH45" s="5"/>
+      <c r="AI45" s="5"/>
+      <c r="AJ45" s="5"/>
+      <c r="AK45" s="5"/>
+      <c r="AL45" s="5"/>
+      <c r="AM45" s="5"/>
+      <c r="AN45" s="5"/>
+      <c r="AO45" s="5"/>
+      <c r="AP45" s="5"/>
+      <c r="AQ45" s="5"/>
+      <c r="AR45" s="5"/>
+      <c r="AS45" s="5"/>
+      <c r="AT45" s="5"/>
+      <c r="AU45" s="5"/>
+      <c r="AV45" s="5"/>
+      <c r="AW45" s="5"/>
+      <c r="AX45" s="5"/>
+      <c r="AY45" s="5"/>
+      <c r="AZ45" s="5"/>
+      <c r="BA45" s="5"/>
+      <c r="BB45" s="5"/>
+      <c r="BC45" s="5"/>
+      <c r="BD45" s="5"/>
+      <c r="BE45" s="28"/>
+      <c r="BF45" s="27"/>
+    </row>
+    <row r="46" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C46" s="6">
         <v>110</v>
@@ -2831,7 +4259,7 @@
         <v>missing</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
@@ -2858,13 +4286,44 @@
       <c r="Z46" s="6"/>
       <c r="AA46" s="6"/>
       <c r="AB46" s="6"/>
-      <c r="AC46" s="3"/>
-      <c r="AD46" s="3"/>
+      <c r="AC46" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD46" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="AE46" s="3"/>
-    </row>
-    <row r="47" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF46" s="28"/>
+      <c r="AG46" s="5"/>
+      <c r="AH46" s="5"/>
+      <c r="AI46" s="5"/>
+      <c r="AJ46" s="5"/>
+      <c r="AK46" s="5"/>
+      <c r="AL46" s="5"/>
+      <c r="AM46" s="5"/>
+      <c r="AN46" s="5"/>
+      <c r="AO46" s="5"/>
+      <c r="AP46" s="5"/>
+      <c r="AQ46" s="5"/>
+      <c r="AR46" s="5"/>
+      <c r="AS46" s="5"/>
+      <c r="AT46" s="5"/>
+      <c r="AU46" s="5"/>
+      <c r="AV46" s="5"/>
+      <c r="AW46" s="5"/>
+      <c r="AX46" s="5"/>
+      <c r="AY46" s="5"/>
+      <c r="AZ46" s="5"/>
+      <c r="BA46" s="5"/>
+      <c r="BB46" s="5"/>
+      <c r="BC46" s="5"/>
+      <c r="BD46" s="5"/>
+      <c r="BE46" s="28"/>
+      <c r="BF46" s="27"/>
+    </row>
+    <row r="47" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C47" s="6">
         <v>111</v>
@@ -2899,13 +4358,42 @@
       <c r="Z47" s="6"/>
       <c r="AA47" s="6"/>
       <c r="AB47" s="6"/>
-      <c r="AC47" s="3"/>
+      <c r="AC47" s="24" t="s">
+        <v>116</v>
+      </c>
       <c r="AD47" s="3"/>
       <c r="AE47" s="3"/>
-    </row>
-    <row r="48" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF47" s="28"/>
+      <c r="AG47" s="5"/>
+      <c r="AH47" s="5"/>
+      <c r="AI47" s="5"/>
+      <c r="AJ47" s="5"/>
+      <c r="AK47" s="5"/>
+      <c r="AL47" s="5"/>
+      <c r="AM47" s="5"/>
+      <c r="AN47" s="5"/>
+      <c r="AO47" s="5"/>
+      <c r="AP47" s="5"/>
+      <c r="AQ47" s="5"/>
+      <c r="AR47" s="5"/>
+      <c r="AS47" s="5"/>
+      <c r="AT47" s="5"/>
+      <c r="AU47" s="5"/>
+      <c r="AV47" s="5"/>
+      <c r="AW47" s="5"/>
+      <c r="AX47" s="5"/>
+      <c r="AY47" s="5"/>
+      <c r="AZ47" s="5"/>
+      <c r="BA47" s="5"/>
+      <c r="BB47" s="5"/>
+      <c r="BC47" s="5"/>
+      <c r="BD47" s="5"/>
+      <c r="BE47" s="28"/>
+      <c r="BF47" s="27"/>
+    </row>
+    <row r="48" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C48" s="6">
         <v>111</v>
@@ -2915,7 +4403,7 @@
         <v>missing</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
@@ -2933,7 +4421,7 @@
       <c r="S48" s="6"/>
       <c r="T48" s="6"/>
       <c r="U48" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V48" s="6"/>
       <c r="W48" s="6"/>
@@ -2942,13 +4430,44 @@
       <c r="Z48" s="6"/>
       <c r="AA48" s="6"/>
       <c r="AB48" s="6"/>
-      <c r="AC48" s="3"/>
-      <c r="AD48" s="3"/>
+      <c r="AC48" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD48" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="AE48" s="3"/>
-    </row>
-    <row r="49" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF48" s="28"/>
+      <c r="AG48" s="5"/>
+      <c r="AH48" s="5"/>
+      <c r="AI48" s="5"/>
+      <c r="AJ48" s="5"/>
+      <c r="AK48" s="5"/>
+      <c r="AL48" s="5"/>
+      <c r="AM48" s="5"/>
+      <c r="AN48" s="5"/>
+      <c r="AO48" s="5"/>
+      <c r="AP48" s="5"/>
+      <c r="AQ48" s="5"/>
+      <c r="AR48" s="5"/>
+      <c r="AS48" s="5"/>
+      <c r="AT48" s="5"/>
+      <c r="AU48" s="5"/>
+      <c r="AV48" s="5"/>
+      <c r="AW48" s="5"/>
+      <c r="AX48" s="5"/>
+      <c r="AY48" s="5"/>
+      <c r="AZ48" s="5"/>
+      <c r="BA48" s="5"/>
+      <c r="BB48" s="5"/>
+      <c r="BC48" s="5"/>
+      <c r="BD48" s="5"/>
+      <c r="BE48" s="28"/>
+      <c r="BF48" s="27"/>
+    </row>
+    <row r="49" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C49" s="6">
         <v>111</v>
@@ -2958,7 +4477,7 @@
         <v>missing</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
@@ -2985,13 +4504,44 @@
       <c r="Z49" s="6"/>
       <c r="AA49" s="6"/>
       <c r="AB49" s="6"/>
-      <c r="AC49" s="3"/>
-      <c r="AD49" s="3"/>
+      <c r="AC49" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD49" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="AE49" s="3"/>
-    </row>
-    <row r="50" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF49" s="28"/>
+      <c r="AG49" s="5"/>
+      <c r="AH49" s="5"/>
+      <c r="AI49" s="5"/>
+      <c r="AJ49" s="5"/>
+      <c r="AK49" s="5"/>
+      <c r="AL49" s="5"/>
+      <c r="AM49" s="5"/>
+      <c r="AN49" s="5"/>
+      <c r="AO49" s="5"/>
+      <c r="AP49" s="5"/>
+      <c r="AQ49" s="5"/>
+      <c r="AR49" s="5"/>
+      <c r="AS49" s="5"/>
+      <c r="AT49" s="5"/>
+      <c r="AU49" s="5"/>
+      <c r="AV49" s="5"/>
+      <c r="AW49" s="5"/>
+      <c r="AX49" s="5"/>
+      <c r="AY49" s="5"/>
+      <c r="AZ49" s="5"/>
+      <c r="BA49" s="5"/>
+      <c r="BB49" s="5"/>
+      <c r="BC49" s="5"/>
+      <c r="BD49" s="5"/>
+      <c r="BE49" s="28"/>
+      <c r="BF49" s="27"/>
+    </row>
+    <row r="50" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C50" s="6">
         <v>112</v>
@@ -3025,22 +4575,51 @@
       <c r="Z50" s="6"/>
       <c r="AA50" s="6"/>
       <c r="AB50" s="6"/>
-      <c r="AC50" s="3"/>
+      <c r="AC50" s="24" t="s">
+        <v>115</v>
+      </c>
       <c r="AD50" s="3"/>
       <c r="AE50" s="3"/>
-    </row>
-    <row r="51" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF50" s="28"/>
+      <c r="AG50" s="5"/>
+      <c r="AH50" s="5"/>
+      <c r="AI50" s="5"/>
+      <c r="AJ50" s="5"/>
+      <c r="AK50" s="5"/>
+      <c r="AL50" s="5"/>
+      <c r="AM50" s="5"/>
+      <c r="AN50" s="5"/>
+      <c r="AO50" s="5"/>
+      <c r="AP50" s="5"/>
+      <c r="AQ50" s="5"/>
+      <c r="AR50" s="5"/>
+      <c r="AS50" s="5"/>
+      <c r="AT50" s="5"/>
+      <c r="AU50" s="5"/>
+      <c r="AV50" s="5"/>
+      <c r="AW50" s="5"/>
+      <c r="AX50" s="5"/>
+      <c r="AY50" s="5"/>
+      <c r="AZ50" s="5"/>
+      <c r="BA50" s="5"/>
+      <c r="BB50" s="5"/>
+      <c r="BC50" s="5"/>
+      <c r="BD50" s="5"/>
+      <c r="BE50" s="28"/>
+      <c r="BF50" s="27"/>
+    </row>
+    <row r="51" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C51" s="6">
         <v>112</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
@@ -3059,7 +4638,7 @@
       <c r="T51" s="6"/>
       <c r="U51" s="6"/>
       <c r="V51" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W51" s="6"/>
       <c r="X51" s="6"/>
@@ -3067,22 +4646,53 @@
       <c r="Z51" s="6"/>
       <c r="AA51" s="6"/>
       <c r="AB51" s="6"/>
-      <c r="AC51" s="3"/>
-      <c r="AD51" s="3"/>
+      <c r="AC51" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD51" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="AE51" s="3"/>
-    </row>
-    <row r="52" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF51" s="28"/>
+      <c r="AG51" s="5"/>
+      <c r="AH51" s="5"/>
+      <c r="AI51" s="5"/>
+      <c r="AJ51" s="5"/>
+      <c r="AK51" s="5"/>
+      <c r="AL51" s="5"/>
+      <c r="AM51" s="5"/>
+      <c r="AN51" s="5"/>
+      <c r="AO51" s="5"/>
+      <c r="AP51" s="5"/>
+      <c r="AQ51" s="5"/>
+      <c r="AR51" s="5"/>
+      <c r="AS51" s="5"/>
+      <c r="AT51" s="5"/>
+      <c r="AU51" s="5"/>
+      <c r="AV51" s="5"/>
+      <c r="AW51" s="5"/>
+      <c r="AX51" s="5"/>
+      <c r="AY51" s="5"/>
+      <c r="AZ51" s="5"/>
+      <c r="BA51" s="5"/>
+      <c r="BB51" s="5"/>
+      <c r="BC51" s="5"/>
+      <c r="BD51" s="5"/>
+      <c r="BE51" s="28"/>
+      <c r="BF51" s="27"/>
+    </row>
+    <row r="52" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C52" s="6">
         <v>112</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
@@ -3109,13 +4719,44 @@
       <c r="Z52" s="6"/>
       <c r="AA52" s="6"/>
       <c r="AB52" s="6"/>
-      <c r="AC52" s="3"/>
-      <c r="AD52" s="3"/>
+      <c r="AC52" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD52" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="AE52" s="3"/>
-    </row>
-    <row r="53" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF52" s="28"/>
+      <c r="AG52" s="5"/>
+      <c r="AH52" s="5"/>
+      <c r="AI52" s="5"/>
+      <c r="AJ52" s="5"/>
+      <c r="AK52" s="5"/>
+      <c r="AL52" s="5"/>
+      <c r="AM52" s="5"/>
+      <c r="AN52" s="5"/>
+      <c r="AO52" s="5"/>
+      <c r="AP52" s="5"/>
+      <c r="AQ52" s="5"/>
+      <c r="AR52" s="5"/>
+      <c r="AS52" s="5"/>
+      <c r="AT52" s="5"/>
+      <c r="AU52" s="5"/>
+      <c r="AV52" s="5"/>
+      <c r="AW52" s="5"/>
+      <c r="AX52" s="5"/>
+      <c r="AY52" s="5"/>
+      <c r="AZ52" s="5"/>
+      <c r="BA52" s="5"/>
+      <c r="BB52" s="5"/>
+      <c r="BC52" s="5"/>
+      <c r="BD52" s="5"/>
+      <c r="BE52" s="28"/>
+      <c r="BF52" s="27"/>
+    </row>
+    <row r="53" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C53" s="6">
         <v>113</v>
@@ -3149,21 +4790,50 @@
       <c r="Z53" s="6"/>
       <c r="AA53" s="6"/>
       <c r="AB53" s="6"/>
-      <c r="AC53" s="3"/>
+      <c r="AC53" s="24" t="s">
+        <v>114</v>
+      </c>
       <c r="AD53" s="3"/>
       <c r="AE53" s="3"/>
-    </row>
-    <row r="54" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF53" s="28"/>
+      <c r="AG53" s="5"/>
+      <c r="AH53" s="5"/>
+      <c r="AI53" s="5"/>
+      <c r="AJ53" s="5"/>
+      <c r="AK53" s="5"/>
+      <c r="AL53" s="5"/>
+      <c r="AM53" s="5"/>
+      <c r="AN53" s="5"/>
+      <c r="AO53" s="5"/>
+      <c r="AP53" s="5"/>
+      <c r="AQ53" s="5"/>
+      <c r="AR53" s="5"/>
+      <c r="AS53" s="5"/>
+      <c r="AT53" s="5"/>
+      <c r="AU53" s="5"/>
+      <c r="AV53" s="5"/>
+      <c r="AW53" s="5"/>
+      <c r="AX53" s="5"/>
+      <c r="AY53" s="5"/>
+      <c r="AZ53" s="5"/>
+      <c r="BA53" s="5"/>
+      <c r="BB53" s="5"/>
+      <c r="BC53" s="5"/>
+      <c r="BD53" s="5"/>
+      <c r="BE53" s="28"/>
+      <c r="BF53" s="27"/>
+    </row>
+    <row r="54" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C54" s="6">
         <v>113</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E54" s="7"/>
+        <v>17</v>
+      </c>
+      <c r="E54" s="19"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
@@ -3182,28 +4852,59 @@
       <c r="U54" s="6"/>
       <c r="V54" s="6"/>
       <c r="W54" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X54" s="6"/>
       <c r="Y54" s="6"/>
       <c r="Z54" s="6"/>
       <c r="AA54" s="6"/>
       <c r="AB54" s="6"/>
-      <c r="AC54" s="3"/>
-      <c r="AD54" s="3"/>
+      <c r="AC54" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD54" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="AE54" s="3"/>
-    </row>
-    <row r="55" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF54" s="28"/>
+      <c r="AG54" s="5"/>
+      <c r="AH54" s="5"/>
+      <c r="AI54" s="5"/>
+      <c r="AJ54" s="5"/>
+      <c r="AK54" s="5"/>
+      <c r="AL54" s="5"/>
+      <c r="AM54" s="5"/>
+      <c r="AN54" s="5"/>
+      <c r="AO54" s="5"/>
+      <c r="AP54" s="5"/>
+      <c r="AQ54" s="5"/>
+      <c r="AR54" s="5"/>
+      <c r="AS54" s="5"/>
+      <c r="AT54" s="5"/>
+      <c r="AU54" s="5"/>
+      <c r="AV54" s="5"/>
+      <c r="AW54" s="5"/>
+      <c r="AX54" s="5"/>
+      <c r="AY54" s="5"/>
+      <c r="AZ54" s="5"/>
+      <c r="BA54" s="5"/>
+      <c r="BB54" s="5"/>
+      <c r="BC54" s="5"/>
+      <c r="BD54" s="5"/>
+      <c r="BE54" s="28"/>
+      <c r="BF54" s="27"/>
+    </row>
+    <row r="55" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B55" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C55" s="6">
         <v>113</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E55" s="7"/>
+        <v>17</v>
+      </c>
+      <c r="E55" s="19"/>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
@@ -3229,13 +4930,44 @@
       <c r="Z55" s="6"/>
       <c r="AA55" s="6"/>
       <c r="AB55" s="6"/>
-      <c r="AC55" s="3"/>
-      <c r="AD55" s="3"/>
+      <c r="AC55" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD55" s="26" t="s">
+        <v>41</v>
+      </c>
       <c r="AE55" s="3"/>
-    </row>
-    <row r="56" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF55" s="28"/>
+      <c r="AG55" s="5"/>
+      <c r="AH55" s="5"/>
+      <c r="AI55" s="5"/>
+      <c r="AJ55" s="5"/>
+      <c r="AK55" s="5"/>
+      <c r="AL55" s="5"/>
+      <c r="AM55" s="5"/>
+      <c r="AN55" s="5"/>
+      <c r="AO55" s="5"/>
+      <c r="AP55" s="5"/>
+      <c r="AQ55" s="5"/>
+      <c r="AR55" s="5"/>
+      <c r="AS55" s="5"/>
+      <c r="AT55" s="5"/>
+      <c r="AU55" s="5"/>
+      <c r="AV55" s="5"/>
+      <c r="AW55" s="5"/>
+      <c r="AX55" s="5"/>
+      <c r="AY55" s="5"/>
+      <c r="AZ55" s="5"/>
+      <c r="BA55" s="5"/>
+      <c r="BB55" s="5"/>
+      <c r="BC55" s="5"/>
+      <c r="BD55" s="5"/>
+      <c r="BE55" s="28"/>
+      <c r="BF55" s="27"/>
+    </row>
+    <row r="56" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C56" s="6">
         <v>118</v>
@@ -3269,22 +5001,51 @@
       <c r="Z56" s="6"/>
       <c r="AA56" s="6"/>
       <c r="AB56" s="6"/>
-      <c r="AC56" s="3"/>
+      <c r="AC56" s="24" t="s">
+        <v>117</v>
+      </c>
       <c r="AD56" s="3"/>
       <c r="AE56" s="3"/>
-    </row>
-    <row r="57" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF56" s="28"/>
+      <c r="AG56" s="5"/>
+      <c r="AH56" s="5"/>
+      <c r="AI56" s="5"/>
+      <c r="AJ56" s="5"/>
+      <c r="AK56" s="5"/>
+      <c r="AL56" s="5"/>
+      <c r="AM56" s="5"/>
+      <c r="AN56" s="5"/>
+      <c r="AO56" s="5"/>
+      <c r="AP56" s="5"/>
+      <c r="AQ56" s="5"/>
+      <c r="AR56" s="5"/>
+      <c r="AS56" s="5"/>
+      <c r="AT56" s="5"/>
+      <c r="AU56" s="5"/>
+      <c r="AV56" s="5"/>
+      <c r="AW56" s="5"/>
+      <c r="AX56" s="5"/>
+      <c r="AY56" s="5"/>
+      <c r="AZ56" s="5"/>
+      <c r="BA56" s="5"/>
+      <c r="BB56" s="5"/>
+      <c r="BC56" s="5"/>
+      <c r="BD56" s="5"/>
+      <c r="BE56" s="28"/>
+      <c r="BF56" s="27"/>
+    </row>
+    <row r="57" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C57" s="6">
         <v>118</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
@@ -3305,28 +5066,59 @@
       <c r="V57" s="6"/>
       <c r="W57" s="6"/>
       <c r="X57" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y57" s="6"/>
       <c r="Z57" s="6"/>
       <c r="AA57" s="6"/>
       <c r="AB57" s="6"/>
-      <c r="AC57" s="3"/>
-      <c r="AD57" s="3"/>
+      <c r="AC57" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD57" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="AE57" s="3"/>
-    </row>
-    <row r="58" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF57" s="28"/>
+      <c r="AG57" s="5"/>
+      <c r="AH57" s="5"/>
+      <c r="AI57" s="5"/>
+      <c r="AJ57" s="5"/>
+      <c r="AK57" s="5"/>
+      <c r="AL57" s="5"/>
+      <c r="AM57" s="5"/>
+      <c r="AN57" s="5"/>
+      <c r="AO57" s="5"/>
+      <c r="AP57" s="5"/>
+      <c r="AQ57" s="5"/>
+      <c r="AR57" s="5"/>
+      <c r="AS57" s="5"/>
+      <c r="AT57" s="5"/>
+      <c r="AU57" s="5"/>
+      <c r="AV57" s="5"/>
+      <c r="AW57" s="5"/>
+      <c r="AX57" s="5"/>
+      <c r="AY57" s="5"/>
+      <c r="AZ57" s="5"/>
+      <c r="BA57" s="5"/>
+      <c r="BB57" s="5"/>
+      <c r="BC57" s="5"/>
+      <c r="BD57" s="5"/>
+      <c r="BE57" s="28"/>
+      <c r="BF57" s="27"/>
+    </row>
+    <row r="58" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C58" s="6">
         <v>118</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
@@ -3353,13 +5145,44 @@
       <c r="Z58" s="6"/>
       <c r="AA58" s="6"/>
       <c r="AB58" s="6"/>
-      <c r="AC58" s="3"/>
-      <c r="AD58" s="3"/>
+      <c r="AC58" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD58" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="AE58" s="3"/>
-    </row>
-    <row r="59" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF58" s="28"/>
+      <c r="AG58" s="5"/>
+      <c r="AH58" s="5"/>
+      <c r="AI58" s="5"/>
+      <c r="AJ58" s="5"/>
+      <c r="AK58" s="5"/>
+      <c r="AL58" s="5"/>
+      <c r="AM58" s="5"/>
+      <c r="AN58" s="5"/>
+      <c r="AO58" s="5"/>
+      <c r="AP58" s="5"/>
+      <c r="AQ58" s="5"/>
+      <c r="AR58" s="5"/>
+      <c r="AS58" s="5"/>
+      <c r="AT58" s="5"/>
+      <c r="AU58" s="5"/>
+      <c r="AV58" s="5"/>
+      <c r="AW58" s="5"/>
+      <c r="AX58" s="5"/>
+      <c r="AY58" s="5"/>
+      <c r="AZ58" s="5"/>
+      <c r="BA58" s="5"/>
+      <c r="BB58" s="5"/>
+      <c r="BC58" s="5"/>
+      <c r="BD58" s="5"/>
+      <c r="BE58" s="28"/>
+      <c r="BF58" s="27"/>
+    </row>
+    <row r="59" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B59" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C59" s="6">
         <v>114</v>
@@ -3394,13 +5217,42 @@
       <c r="Z59" s="6"/>
       <c r="AA59" s="6"/>
       <c r="AB59" s="6"/>
-      <c r="AC59" s="3"/>
+      <c r="AC59" s="24" t="s">
+        <v>119</v>
+      </c>
       <c r="AD59" s="3"/>
       <c r="AE59" s="3"/>
-    </row>
-    <row r="60" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF59" s="28"/>
+      <c r="AG59" s="5"/>
+      <c r="AH59" s="5"/>
+      <c r="AI59" s="5"/>
+      <c r="AJ59" s="5"/>
+      <c r="AK59" s="5"/>
+      <c r="AL59" s="5"/>
+      <c r="AM59" s="5"/>
+      <c r="AN59" s="5"/>
+      <c r="AO59" s="5"/>
+      <c r="AP59" s="5"/>
+      <c r="AQ59" s="5"/>
+      <c r="AR59" s="5"/>
+      <c r="AS59" s="5"/>
+      <c r="AT59" s="5"/>
+      <c r="AU59" s="5"/>
+      <c r="AV59" s="5"/>
+      <c r="AW59" s="5"/>
+      <c r="AX59" s="5"/>
+      <c r="AY59" s="5"/>
+      <c r="AZ59" s="5"/>
+      <c r="BA59" s="5"/>
+      <c r="BB59" s="5"/>
+      <c r="BC59" s="5"/>
+      <c r="BD59" s="5"/>
+      <c r="BE59" s="28"/>
+      <c r="BF59" s="27"/>
+    </row>
+    <row r="60" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B60" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C60" s="6">
         <v>114</v>
@@ -3410,7 +5262,7 @@
         <v>missing</v>
       </c>
       <c r="E60" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
@@ -3432,18 +5284,49 @@
       <c r="W60" s="6"/>
       <c r="X60" s="6"/>
       <c r="Y60" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Z60" s="6"/>
       <c r="AA60" s="6"/>
       <c r="AB60" s="6"/>
-      <c r="AC60" s="3"/>
-      <c r="AD60" s="3"/>
+      <c r="AC60" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD60" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="AE60" s="3"/>
-    </row>
-    <row r="61" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF60" s="28"/>
+      <c r="AG60" s="5"/>
+      <c r="AH60" s="5"/>
+      <c r="AI60" s="5"/>
+      <c r="AJ60" s="5"/>
+      <c r="AK60" s="5"/>
+      <c r="AL60" s="5"/>
+      <c r="AM60" s="5"/>
+      <c r="AN60" s="5"/>
+      <c r="AO60" s="5"/>
+      <c r="AP60" s="5"/>
+      <c r="AQ60" s="5"/>
+      <c r="AR60" s="5"/>
+      <c r="AS60" s="5"/>
+      <c r="AT60" s="5"/>
+      <c r="AU60" s="5"/>
+      <c r="AV60" s="5"/>
+      <c r="AW60" s="5"/>
+      <c r="AX60" s="5"/>
+      <c r="AY60" s="5"/>
+      <c r="AZ60" s="5"/>
+      <c r="BA60" s="5"/>
+      <c r="BB60" s="5"/>
+      <c r="BC60" s="5"/>
+      <c r="BD60" s="5"/>
+      <c r="BE60" s="28"/>
+      <c r="BF60" s="27"/>
+    </row>
+    <row r="61" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C61" s="6">
         <v>114</v>
@@ -3453,7 +5336,7 @@
         <v>missing</v>
       </c>
       <c r="E61" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
@@ -3480,13 +5363,44 @@
       <c r="Z61" s="6"/>
       <c r="AA61" s="6"/>
       <c r="AB61" s="6"/>
-      <c r="AC61" s="3"/>
-      <c r="AD61" s="3"/>
+      <c r="AC61" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD61" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="AE61" s="3"/>
-    </row>
-    <row r="62" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF61" s="28"/>
+      <c r="AG61" s="5"/>
+      <c r="AH61" s="5"/>
+      <c r="AI61" s="5"/>
+      <c r="AJ61" s="5"/>
+      <c r="AK61" s="5"/>
+      <c r="AL61" s="5"/>
+      <c r="AM61" s="5"/>
+      <c r="AN61" s="5"/>
+      <c r="AO61" s="5"/>
+      <c r="AP61" s="5"/>
+      <c r="AQ61" s="5"/>
+      <c r="AR61" s="5"/>
+      <c r="AS61" s="5"/>
+      <c r="AT61" s="5"/>
+      <c r="AU61" s="5"/>
+      <c r="AV61" s="5"/>
+      <c r="AW61" s="5"/>
+      <c r="AX61" s="5"/>
+      <c r="AY61" s="5"/>
+      <c r="AZ61" s="5"/>
+      <c r="BA61" s="5"/>
+      <c r="BB61" s="5"/>
+      <c r="BC61" s="5"/>
+      <c r="BD61" s="5"/>
+      <c r="BE61" s="28"/>
+      <c r="BF61" s="27"/>
+    </row>
+    <row r="62" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C62" s="6">
         <v>115</v>
@@ -3521,13 +5435,42 @@
       </c>
       <c r="AA62" s="6"/>
       <c r="AB62" s="6"/>
-      <c r="AC62" s="3"/>
+      <c r="AC62" s="24" t="s">
+        <v>118</v>
+      </c>
       <c r="AD62" s="3"/>
       <c r="AE62" s="3"/>
-    </row>
-    <row r="63" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF62" s="28"/>
+      <c r="AG62" s="5"/>
+      <c r="AH62" s="5"/>
+      <c r="AI62" s="5"/>
+      <c r="AJ62" s="5"/>
+      <c r="AK62" s="5"/>
+      <c r="AL62" s="5"/>
+      <c r="AM62" s="5"/>
+      <c r="AN62" s="5"/>
+      <c r="AO62" s="5"/>
+      <c r="AP62" s="5"/>
+      <c r="AQ62" s="5"/>
+      <c r="AR62" s="5"/>
+      <c r="AS62" s="5"/>
+      <c r="AT62" s="5"/>
+      <c r="AU62" s="5"/>
+      <c r="AV62" s="5"/>
+      <c r="AW62" s="5"/>
+      <c r="AX62" s="5"/>
+      <c r="AY62" s="5"/>
+      <c r="AZ62" s="5"/>
+      <c r="BA62" s="5"/>
+      <c r="BB62" s="5"/>
+      <c r="BC62" s="5"/>
+      <c r="BD62" s="5"/>
+      <c r="BE62" s="28"/>
+      <c r="BF62" s="27"/>
+    </row>
+    <row r="63" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C63" s="6">
         <v>115</v>
@@ -3537,7 +5480,7 @@
         <v>missing</v>
       </c>
       <c r="E63" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
@@ -3560,17 +5503,48 @@
       <c r="X63" s="6"/>
       <c r="Y63" s="6"/>
       <c r="Z63" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA63" s="6"/>
       <c r="AB63" s="6"/>
-      <c r="AC63" s="3"/>
-      <c r="AD63" s="3"/>
+      <c r="AC63" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD63" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="AE63" s="3"/>
-    </row>
-    <row r="64" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF63" s="28"/>
+      <c r="AG63" s="5"/>
+      <c r="AH63" s="5"/>
+      <c r="AI63" s="5"/>
+      <c r="AJ63" s="5"/>
+      <c r="AK63" s="5"/>
+      <c r="AL63" s="5"/>
+      <c r="AM63" s="5"/>
+      <c r="AN63" s="5"/>
+      <c r="AO63" s="5"/>
+      <c r="AP63" s="5"/>
+      <c r="AQ63" s="5"/>
+      <c r="AR63" s="5"/>
+      <c r="AS63" s="5"/>
+      <c r="AT63" s="5"/>
+      <c r="AU63" s="5"/>
+      <c r="AV63" s="5"/>
+      <c r="AW63" s="5"/>
+      <c r="AX63" s="5"/>
+      <c r="AY63" s="5"/>
+      <c r="AZ63" s="5"/>
+      <c r="BA63" s="5"/>
+      <c r="BB63" s="5"/>
+      <c r="BC63" s="5"/>
+      <c r="BD63" s="5"/>
+      <c r="BE63" s="28"/>
+      <c r="BF63" s="27"/>
+    </row>
+    <row r="64" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C64" s="6">
         <v>115</v>
@@ -3580,7 +5554,7 @@
         <v>missing</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
@@ -3607,13 +5581,44 @@
       </c>
       <c r="AA64" s="6"/>
       <c r="AB64" s="6"/>
-      <c r="AC64" s="3"/>
-      <c r="AD64" s="3"/>
+      <c r="AC64" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD64" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="AE64" s="3"/>
-    </row>
-    <row r="65" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF64" s="28"/>
+      <c r="AG64" s="5"/>
+      <c r="AH64" s="5"/>
+      <c r="AI64" s="5"/>
+      <c r="AJ64" s="5"/>
+      <c r="AK64" s="5"/>
+      <c r="AL64" s="5"/>
+      <c r="AM64" s="5"/>
+      <c r="AN64" s="5"/>
+      <c r="AO64" s="5"/>
+      <c r="AP64" s="5"/>
+      <c r="AQ64" s="5"/>
+      <c r="AR64" s="5"/>
+      <c r="AS64" s="5"/>
+      <c r="AT64" s="5"/>
+      <c r="AU64" s="5"/>
+      <c r="AV64" s="5"/>
+      <c r="AW64" s="5"/>
+      <c r="AX64" s="5"/>
+      <c r="AY64" s="5"/>
+      <c r="AZ64" s="5"/>
+      <c r="BA64" s="5"/>
+      <c r="BB64" s="5"/>
+      <c r="BC64" s="5"/>
+      <c r="BD64" s="5"/>
+      <c r="BE64" s="28"/>
+      <c r="BF64" s="27"/>
+    </row>
+    <row r="65" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C65" s="6">
         <v>116</v>
@@ -3648,13 +5653,42 @@
         <v>1</v>
       </c>
       <c r="AB65" s="6"/>
-      <c r="AC65" s="3"/>
+      <c r="AC65" s="24" t="s">
+        <v>120</v>
+      </c>
       <c r="AD65" s="3"/>
       <c r="AE65" s="3"/>
-    </row>
-    <row r="66" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF65" s="28"/>
+      <c r="AG65" s="5"/>
+      <c r="AH65" s="5"/>
+      <c r="AI65" s="5"/>
+      <c r="AJ65" s="5"/>
+      <c r="AK65" s="5"/>
+      <c r="AL65" s="5"/>
+      <c r="AM65" s="5"/>
+      <c r="AN65" s="5"/>
+      <c r="AO65" s="5"/>
+      <c r="AP65" s="5"/>
+      <c r="AQ65" s="5"/>
+      <c r="AR65" s="5"/>
+      <c r="AS65" s="5"/>
+      <c r="AT65" s="5"/>
+      <c r="AU65" s="5"/>
+      <c r="AV65" s="5"/>
+      <c r="AW65" s="5"/>
+      <c r="AX65" s="5"/>
+      <c r="AY65" s="5"/>
+      <c r="AZ65" s="5"/>
+      <c r="BA65" s="5"/>
+      <c r="BB65" s="5"/>
+      <c r="BC65" s="5"/>
+      <c r="BD65" s="5"/>
+      <c r="BE65" s="28"/>
+      <c r="BF65" s="27"/>
+    </row>
+    <row r="66" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B66" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C66" s="6">
         <v>116</v>
@@ -3689,23 +5723,52 @@
         <v>0</v>
       </c>
       <c r="AB66" s="6"/>
-      <c r="AC66" s="3"/>
+      <c r="AC66" s="24" t="s">
+        <v>121</v>
+      </c>
       <c r="AD66" s="3"/>
       <c r="AE66" s="3"/>
-    </row>
-    <row r="67" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF66" s="28"/>
+      <c r="AG66" s="5"/>
+      <c r="AH66" s="5"/>
+      <c r="AI66" s="5"/>
+      <c r="AJ66" s="5"/>
+      <c r="AK66" s="5"/>
+      <c r="AL66" s="5"/>
+      <c r="AM66" s="5"/>
+      <c r="AN66" s="5"/>
+      <c r="AO66" s="5"/>
+      <c r="AP66" s="5"/>
+      <c r="AQ66" s="5"/>
+      <c r="AR66" s="5"/>
+      <c r="AS66" s="5"/>
+      <c r="AT66" s="5"/>
+      <c r="AU66" s="5"/>
+      <c r="AV66" s="5"/>
+      <c r="AW66" s="5"/>
+      <c r="AX66" s="5"/>
+      <c r="AY66" s="5"/>
+      <c r="AZ66" s="5"/>
+      <c r="BA66" s="5"/>
+      <c r="BB66" s="5"/>
+      <c r="BC66" s="5"/>
+      <c r="BD66" s="5"/>
+      <c r="BE66" s="28"/>
+      <c r="BF66" s="27"/>
+    </row>
+    <row r="67" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B67" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C67" s="6">
         <v>116</v>
       </c>
-      <c r="D67" s="6" t="str">
+      <c r="D67" s="20" t="str">
         <f>IF(AA67= "-","missing",AA67)</f>
         <v>missing</v>
       </c>
       <c r="E67" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
@@ -3729,16 +5792,47 @@
       <c r="Y67" s="6"/>
       <c r="Z67" s="6"/>
       <c r="AA67" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AB67" s="6"/>
-      <c r="AC67" s="3"/>
-      <c r="AD67" s="3"/>
+      <c r="AC67" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD67" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="AE67" s="3"/>
-    </row>
-    <row r="68" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF67" s="28"/>
+      <c r="AG67" s="5"/>
+      <c r="AH67" s="5"/>
+      <c r="AI67" s="5"/>
+      <c r="AJ67" s="5"/>
+      <c r="AK67" s="5"/>
+      <c r="AL67" s="5"/>
+      <c r="AM67" s="5"/>
+      <c r="AN67" s="5"/>
+      <c r="AO67" s="5"/>
+      <c r="AP67" s="5"/>
+      <c r="AQ67" s="5"/>
+      <c r="AR67" s="5"/>
+      <c r="AS67" s="5"/>
+      <c r="AT67" s="5"/>
+      <c r="AU67" s="5"/>
+      <c r="AV67" s="5"/>
+      <c r="AW67" s="5"/>
+      <c r="AX67" s="5"/>
+      <c r="AY67" s="5"/>
+      <c r="AZ67" s="5"/>
+      <c r="BA67" s="5"/>
+      <c r="BB67" s="5"/>
+      <c r="BC67" s="5"/>
+      <c r="BD67" s="5"/>
+      <c r="BE67" s="28"/>
+      <c r="BF67" s="27"/>
+    </row>
+    <row r="68" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B68" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C68" s="6">
         <v>117</v>
@@ -3773,13 +5867,42 @@
       <c r="AB68" s="6">
         <v>200</v>
       </c>
-      <c r="AC68" s="3"/>
+      <c r="AC68" s="24" t="s">
+        <v>116</v>
+      </c>
       <c r="AD68" s="3"/>
       <c r="AE68" s="3"/>
-    </row>
-    <row r="69" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF68" s="28"/>
+      <c r="AG68" s="5"/>
+      <c r="AH68" s="5"/>
+      <c r="AI68" s="5"/>
+      <c r="AJ68" s="5"/>
+      <c r="AK68" s="5"/>
+      <c r="AL68" s="5"/>
+      <c r="AM68" s="5"/>
+      <c r="AN68" s="5"/>
+      <c r="AO68" s="5"/>
+      <c r="AP68" s="5"/>
+      <c r="AQ68" s="5"/>
+      <c r="AR68" s="5"/>
+      <c r="AS68" s="5"/>
+      <c r="AT68" s="5"/>
+      <c r="AU68" s="5"/>
+      <c r="AV68" s="5"/>
+      <c r="AW68" s="5"/>
+      <c r="AX68" s="5"/>
+      <c r="AY68" s="5"/>
+      <c r="AZ68" s="5"/>
+      <c r="BA68" s="5"/>
+      <c r="BB68" s="5"/>
+      <c r="BC68" s="5"/>
+      <c r="BD68" s="5"/>
+      <c r="BE68" s="28"/>
+      <c r="BF68" s="27"/>
+    </row>
+    <row r="69" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B69" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C69" s="6">
         <v>117</v>
@@ -3789,7 +5912,7 @@
         <v>missing</v>
       </c>
       <c r="E69" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
@@ -3814,15 +5937,46 @@
       <c r="Z69" s="6"/>
       <c r="AA69" s="6"/>
       <c r="AB69" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC69" s="3"/>
-      <c r="AD69" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="AC69" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD69" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="AE69" s="3"/>
-    </row>
-    <row r="70" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF69" s="28"/>
+      <c r="AG69" s="5"/>
+      <c r="AH69" s="5"/>
+      <c r="AI69" s="5"/>
+      <c r="AJ69" s="5"/>
+      <c r="AK69" s="5"/>
+      <c r="AL69" s="5"/>
+      <c r="AM69" s="5"/>
+      <c r="AN69" s="5"/>
+      <c r="AO69" s="5"/>
+      <c r="AP69" s="5"/>
+      <c r="AQ69" s="5"/>
+      <c r="AR69" s="5"/>
+      <c r="AS69" s="5"/>
+      <c r="AT69" s="5"/>
+      <c r="AU69" s="5"/>
+      <c r="AV69" s="5"/>
+      <c r="AW69" s="5"/>
+      <c r="AX69" s="5"/>
+      <c r="AY69" s="5"/>
+      <c r="AZ69" s="5"/>
+      <c r="BA69" s="5"/>
+      <c r="BB69" s="5"/>
+      <c r="BC69" s="5"/>
+      <c r="BD69" s="5"/>
+      <c r="BE69" s="28"/>
+      <c r="BF69" s="27"/>
+    </row>
+    <row r="70" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B70" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C70" s="16">
         <v>117</v>
@@ -3832,7 +5986,7 @@
         <v>missing</v>
       </c>
       <c r="E70" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F70" s="16"/>
       <c r="G70" s="16"/>
@@ -3859,11 +6013,42 @@
       <c r="AB70" s="16">
         <v>-600</v>
       </c>
-      <c r="AC70" s="11"/>
-      <c r="AD70" s="11"/>
+      <c r="AC70" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD70" s="11" t="s">
+        <v>123</v>
+      </c>
       <c r="AE70" s="11"/>
-    </row>
-    <row r="71" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AF70" s="28"/>
+      <c r="AG70" s="5"/>
+      <c r="AH70" s="5"/>
+      <c r="AI70" s="5"/>
+      <c r="AJ70" s="5"/>
+      <c r="AK70" s="5"/>
+      <c r="AL70" s="5"/>
+      <c r="AM70" s="5"/>
+      <c r="AN70" s="5"/>
+      <c r="AO70" s="5"/>
+      <c r="AP70" s="5"/>
+      <c r="AQ70" s="5"/>
+      <c r="AR70" s="5"/>
+      <c r="AS70" s="5"/>
+      <c r="AT70" s="5"/>
+      <c r="AU70" s="5"/>
+      <c r="AV70" s="5"/>
+      <c r="AW70" s="5"/>
+      <c r="AX70" s="5"/>
+      <c r="AY70" s="5"/>
+      <c r="AZ70" s="5"/>
+      <c r="BA70" s="5"/>
+      <c r="BB70" s="5"/>
+      <c r="BC70" s="5"/>
+      <c r="BD70" s="5"/>
+      <c r="BE70" s="28"/>
+      <c r="BF70" s="27"/>
+    </row>
+    <row r="71" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B71" s="13"/>
       <c r="C71" s="13"/>
       <c r="D71" s="13"/>
@@ -3894,8 +6079,9 @@
       <c r="AC71" s="13"/>
       <c r="AD71" s="13"/>
       <c r="AE71" s="13"/>
-    </row>
-    <row r="72" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="BC71" s="1"/>
+    </row>
+    <row r="72" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
       <c r="D72" s="12"/>
@@ -3926,8 +6112,9 @@
       <c r="AC72" s="12"/>
       <c r="AD72" s="12"/>
       <c r="AE72" s="12"/>
-    </row>
-    <row r="73" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="BC72" s="1"/>
+    </row>
+    <row r="73" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
       <c r="D73" s="12"/>
@@ -3959,7 +6146,7 @@
       <c r="AD73" s="12"/>
       <c r="AE73" s="12"/>
     </row>
-    <row r="74" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
@@ -3991,7 +6178,7 @@
       <c r="AD74" s="12"/>
       <c r="AE74" s="12"/>
     </row>
-    <row r="75" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B75" s="12"/>
       <c r="C75" s="12"/>
       <c r="D75" s="12"/>
@@ -4023,7 +6210,7 @@
       <c r="AD75" s="12"/>
       <c r="AE75" s="12"/>
     </row>
-    <row r="76" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B76" s="12"/>
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
@@ -4055,7 +6242,7 @@
       <c r="AD76" s="12"/>
       <c r="AE76" s="12"/>
     </row>
-    <row r="77" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
       <c r="D77" s="12"/>
@@ -4087,7 +6274,7 @@
       <c r="AD77" s="12"/>
       <c r="AE77" s="12"/>
     </row>
-    <row r="78" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B78" s="12"/>
       <c r="C78" s="12"/>
       <c r="D78" s="12"/>
@@ -4119,7 +6306,7 @@
       <c r="AD78" s="12"/>
       <c r="AE78" s="12"/>
     </row>
-    <row r="79" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B79" s="12"/>
       <c r="C79" s="12"/>
       <c r="D79" s="12"/>
@@ -4151,7 +6338,7 @@
       <c r="AD79" s="12"/>
       <c r="AE79" s="12"/>
     </row>
-    <row r="80" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B80" s="12"/>
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
@@ -4183,7 +6370,7 @@
       <c r="AD80" s="12"/>
       <c r="AE80" s="12"/>
     </row>
-    <row r="81" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B81" s="12"/>
       <c r="C81" s="12"/>
       <c r="D81" s="12"/>

</xml_diff>